<commit_message>
Updated Budget_Calculator.xlsx & Navigation Bar is done & Added Footer
</commit_message>
<xml_diff>
--- a/Event Organizer App/Algorithms/Budget_Calculator.xlsx
+++ b/Event Organizer App/Algorithms/Budget_Calculator.xlsx
@@ -8,22 +8,26 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CabinApp\Cabana_app\Event Organizer App\Algorithms\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95DCF957-2F20-40FA-97CD-0ED65F55A179}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53A965A5-2509-44A5-833E-DC62B9B33FD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{73935AE9-622C-41E0-9B02-D732681E28C4}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="4" xr2:uid="{73935AE9-622C-41E0-9B02-D732681E28C4}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
     <sheet name="DateVoting" sheetId="9" r:id="rId2"/>
     <sheet name="Participation List" sheetId="8" r:id="rId3"/>
-    <sheet name="Finance Report" sheetId="2" r:id="rId4"/>
-    <sheet name="Location" sheetId="3" r:id="rId5"/>
-    <sheet name="Transport" sheetId="4" r:id="rId6"/>
-    <sheet name="Meals &amp; Drinks" sheetId="7" r:id="rId7"/>
-    <sheet name="Activities" sheetId="6" r:id="rId8"/>
-    <sheet name="DJ &amp; Entertainment" sheetId="5" r:id="rId9"/>
+    <sheet name="Sheet1" sheetId="10" r:id="rId4"/>
+    <sheet name="Finance Report" sheetId="2" r:id="rId5"/>
+    <sheet name="Location" sheetId="3" r:id="rId6"/>
+    <sheet name="Transport" sheetId="4" r:id="rId7"/>
+    <sheet name="Meals &amp; Drinks" sheetId="7" r:id="rId8"/>
+    <sheet name="Activities" sheetId="6" r:id="rId9"/>
+    <sheet name="DJ &amp; Entertainment" sheetId="5" r:id="rId10"/>
   </sheets>
-  <calcPr calcId="191029" concurrentCalc="0"/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Participation List'!$A$2:$F$32</definedName>
+  </definedNames>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -43,8 +47,30 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="571" uniqueCount="180">
   <si>
     <t>Buget</t>
   </si>
@@ -470,6 +496,120 @@
   </si>
   <si>
     <t>Autocar Mic?</t>
+  </si>
+  <si>
+    <t>Data</t>
+  </si>
+  <si>
+    <t>Catering</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Autocare</t>
+  </si>
+  <si>
+    <t>Vehicul Personal</t>
+  </si>
+  <si>
+    <t>Alergii</t>
+  </si>
+  <si>
+    <t>Participanti Eveniment</t>
+  </si>
+  <si>
+    <t>27-29 Octombrie</t>
+  </si>
+  <si>
+    <t>10-13 Septembrie</t>
+  </si>
+  <si>
+    <t>18-21 Septembrie</t>
+  </si>
+  <si>
+    <t>particapnt 1</t>
+  </si>
+  <si>
+    <t>vegan</t>
+  </si>
+  <si>
+    <t>transport</t>
+  </si>
+  <si>
+    <t>alergii</t>
+  </si>
+  <si>
+    <t>nu</t>
+  </si>
+  <si>
+    <t>propriu</t>
+  </si>
+  <si>
+    <t>+</t>
+  </si>
+  <si>
+    <t>Add</t>
+  </si>
+  <si>
+    <t>Numele Tau</t>
+  </si>
+  <si>
+    <t>click to vote</t>
+  </si>
+  <si>
+    <t>voted</t>
+  </si>
+  <si>
+    <t>Next -&gt;</t>
+  </si>
+  <si>
+    <t>Creare Tabel</t>
+  </si>
+  <si>
+    <t>Nr. Max participanti</t>
+  </si>
+  <si>
+    <t>27-31 Jun</t>
+  </si>
+  <si>
+    <t>20-23 Jun</t>
+  </si>
+  <si>
+    <t>Data 1</t>
+  </si>
+  <si>
+    <t>Data 2</t>
+  </si>
+  <si>
+    <t>Nume</t>
+  </si>
+  <si>
+    <t>Website</t>
+  </si>
+  <si>
+    <t>https://travelminit.ro/atrium-panoramic-hotel-spa-predeal?ref=list&amp;adults=2&amp;provision=2&amp;listIndex=0</t>
+  </si>
+  <si>
+    <t>Voteaza</t>
+  </si>
+  <si>
+    <t>Anuleaza</t>
+  </si>
+  <si>
+    <t>Popescu Alexandru</t>
+  </si>
+  <si>
+    <t>Guest</t>
+  </si>
+  <si>
+    <t>Organizer</t>
+  </si>
+  <si>
+    <t>15-18 Jun</t>
+  </si>
+  <si>
+    <t>Numar voturi:</t>
   </si>
 </sst>
 </file>
@@ -483,7 +623,7 @@
     <numFmt numFmtId="166" formatCode="[$-418]d\ mmmm\ yyyy;@"/>
     <numFmt numFmtId="167" formatCode="[$-409]h:mm\ AM/PM;@"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color theme="1"/>
@@ -522,8 +662,51 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="24"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="12">
+  <fills count="19">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -590,8 +773,49 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="28">
+  <borders count="46">
     <border>
       <left/>
       <right/>
@@ -974,13 +1198,237 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFFF0000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFFF0000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFFF0000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFFF0000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFFF0000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFFF0000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFFF0000"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FFFF0000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="85">
+  <cellXfs count="156">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1203,6 +1651,9 @@
     <xf numFmtId="167" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1230,9 +1681,181 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="4" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="36" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="29" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="5">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
+    <cellStyle name="Good 2" xfId="3" xr:uid="{F1AEC037-A6C7-45C2-AF82-E8F5527519DF}"/>
+    <cellStyle name="Hyperlink" xfId="4" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
@@ -1308,9 +1931,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1348,7 +1971,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1454,7 +2077,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1596,7 +2219,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1675,20 +2298,20 @@
         <v>10000</v>
       </c>
       <c r="D2" s="45"/>
-      <c r="E2" s="76" t="s">
+      <c r="E2" s="77" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="77"/>
+      <c r="F2" s="78"/>
       <c r="G2" s="45"/>
-      <c r="H2" s="76" t="s">
+      <c r="H2" s="77" t="s">
         <v>9</v>
       </c>
-      <c r="I2" s="77"/>
+      <c r="I2" s="78"/>
       <c r="J2" s="45"/>
-      <c r="K2" s="76" t="s">
+      <c r="K2" s="77" t="s">
         <v>10</v>
       </c>
-      <c r="L2" s="77"/>
+      <c r="L2" s="78"/>
       <c r="P2" s="7" t="s">
         <v>13</v>
       </c>
@@ -2740,11 +3363,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1510B56F-643F-41A2-A11C-FA7DE12E9408}">
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9F22359-FC7F-4C60-A43A-F5055E3A7BE0}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:C3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <sheetData/>
@@ -2752,641 +3377,1967 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D29C6C0-1AA5-4518-814D-180997663027}">
-  <dimension ref="A1:I32"/>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1510B56F-643F-41A2-A11C-FA7DE12E9408}">
+  <dimension ref="A1:Z42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="T5" sqref="T5"/>
+    <sheetView topLeftCell="J8" workbookViewId="0">
+      <selection activeCell="X16" sqref="X16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="21.5546875" customWidth="1"/>
-    <col min="3" max="3" width="6.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="16.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="23.5546875" customWidth="1"/>
-    <col min="8" max="8" width="8.88671875" customWidth="1"/>
-    <col min="9" max="9" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="3" width="19.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="35.88671875" customWidth="1"/>
+    <col min="8" max="10" width="19.21875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.33203125" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="21.5546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="15.33203125" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="16.77734375" bestFit="1" customWidth="1"/>
+    <col min="20" max="21" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="16.77734375" bestFit="1" customWidth="1"/>
+    <col min="25" max="26" width="9.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="80" t="s">
+    <row r="1" spans="1:26" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="89" t="s">
+        <v>149</v>
+      </c>
+      <c r="B1" s="89" t="s">
+        <v>150</v>
+      </c>
+      <c r="C1" s="89" t="s">
+        <v>151</v>
+      </c>
+      <c r="D1" s="99" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="95" t="str" cm="1">
+        <f t="array" ref="F1">INDEX($S$19:$U$19,0,MATCH(MAX($S16:$U16),$S16:$U16,0))</f>
+        <v>15-18 Jun</v>
+      </c>
+      <c r="H1" s="89" t="s">
+        <v>149</v>
+      </c>
+      <c r="I1" s="89" t="s">
+        <v>150</v>
+      </c>
+      <c r="J1" s="89" t="s">
+        <v>151</v>
+      </c>
+      <c r="K1" s="103" t="s">
+        <v>2</v>
+      </c>
+      <c r="M1" s="89" t="s">
+        <v>149</v>
+      </c>
+      <c r="N1" s="89" t="s">
+        <v>150</v>
+      </c>
+      <c r="O1" s="89" t="s">
+        <v>151</v>
+      </c>
+      <c r="P1" s="104" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q1" s="106" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="2" spans="1:26" ht="13.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="87" t="s">
+        <v>115</v>
+      </c>
+      <c r="B2" s="87"/>
+      <c r="C2" s="87" t="s">
+        <v>115</v>
+      </c>
+      <c r="D2" s="66" t="s">
+        <v>133</v>
+      </c>
+      <c r="F2" s="96"/>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2" s="101" t="s">
+        <v>115</v>
+      </c>
+      <c r="I2" s="101"/>
+      <c r="J2" s="101"/>
+      <c r="K2" s="102" t="s">
+        <v>133</v>
+      </c>
+      <c r="M2" s="110" t="s">
+        <v>162</v>
+      </c>
+      <c r="N2" s="110" t="s">
+        <v>161</v>
+      </c>
+      <c r="O2" s="110" t="s">
+        <v>161</v>
+      </c>
+      <c r="P2" s="105" t="s">
+        <v>133</v>
+      </c>
+      <c r="Q2" s="107"/>
+    </row>
+    <row r="3" spans="1:26" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="87" t="s">
+        <v>116</v>
+      </c>
+      <c r="B3" s="87" t="s">
+        <v>116</v>
+      </c>
+      <c r="C3" s="90"/>
+      <c r="D3" s="66" t="s">
+        <v>133</v>
+      </c>
+      <c r="F3" s="96"/>
+      <c r="G3">
+        <v>2</v>
+      </c>
+      <c r="H3" s="87"/>
+      <c r="I3" s="87"/>
+      <c r="J3" s="90"/>
+      <c r="K3" s="66"/>
+    </row>
+    <row r="4" spans="1:26" ht="13.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="87" t="s">
+        <v>117</v>
+      </c>
+      <c r="B4" s="87"/>
+      <c r="C4" s="87" t="s">
+        <v>117</v>
+      </c>
+      <c r="D4" s="66" t="s">
+        <v>133</v>
+      </c>
+      <c r="F4" s="96"/>
+      <c r="G4">
+        <v>3</v>
+      </c>
+      <c r="H4" s="87"/>
+      <c r="I4" s="87"/>
+      <c r="J4" s="87"/>
+      <c r="K4" s="66"/>
+      <c r="M4" s="89" t="s">
+        <v>170</v>
+      </c>
+      <c r="N4" s="89" t="s">
+        <v>2</v>
+      </c>
+      <c r="O4" s="89" t="s">
+        <v>56</v>
+      </c>
+      <c r="P4" s="104" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q4" s="89" t="s">
+        <v>147</v>
+      </c>
+      <c r="R4" s="106" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" ht="13.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="87"/>
+      <c r="B5" s="87" t="s">
+        <v>118</v>
+      </c>
+      <c r="C5" s="91"/>
+      <c r="D5" s="66" t="s">
+        <v>132</v>
+      </c>
+      <c r="F5" s="96"/>
+      <c r="G5">
+        <v>4</v>
+      </c>
+      <c r="H5" s="87"/>
+      <c r="I5" s="87"/>
+      <c r="J5" s="91"/>
+      <c r="K5" s="66"/>
+      <c r="M5" s="110" t="str">
+        <f>M11</f>
+        <v>Alex Popescu</v>
+      </c>
+      <c r="N5" s="110" t="s">
+        <v>133</v>
+      </c>
+      <c r="O5" s="110" t="s">
+        <v>156</v>
+      </c>
+      <c r="P5" s="105" t="s">
+        <v>133</v>
+      </c>
+      <c r="Q5" s="110" t="s">
+        <v>156</v>
+      </c>
+      <c r="R5" s="107"/>
+    </row>
+    <row r="6" spans="1:26" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="87" t="s">
+        <v>119</v>
+      </c>
+      <c r="B6" s="87"/>
+      <c r="C6" s="87" t="s">
+        <v>119</v>
+      </c>
+      <c r="D6" s="66" t="s">
+        <v>133</v>
+      </c>
+      <c r="F6" s="96"/>
+      <c r="G6">
+        <v>5</v>
+      </c>
+      <c r="H6" s="87"/>
+      <c r="I6" s="87"/>
+      <c r="J6" s="87"/>
+      <c r="K6" s="66"/>
+    </row>
+    <row r="7" spans="1:26" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="87" t="s">
+        <v>120</v>
+      </c>
+      <c r="B7" s="87" t="s">
+        <v>120</v>
+      </c>
+      <c r="C7" s="87" t="s">
+        <v>120</v>
+      </c>
+      <c r="D7" s="66" t="s">
+        <v>133</v>
+      </c>
+      <c r="F7" s="96"/>
+      <c r="G7">
+        <v>6</v>
+      </c>
+      <c r="H7" s="87"/>
+      <c r="I7" s="87"/>
+      <c r="J7" s="87"/>
+      <c r="K7" s="66"/>
+    </row>
+    <row r="8" spans="1:26" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="87" t="s">
+        <v>121</v>
+      </c>
+      <c r="B8" s="87" t="s">
+        <v>121</v>
+      </c>
+      <c r="C8" s="91"/>
+      <c r="D8" s="66" t="s">
+        <v>133</v>
+      </c>
+      <c r="F8" s="96"/>
+      <c r="G8">
+        <v>7</v>
+      </c>
+      <c r="H8" s="87"/>
+      <c r="I8" s="87"/>
+      <c r="J8" s="91"/>
+      <c r="K8" s="66"/>
+    </row>
+    <row r="9" spans="1:26" ht="13.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="87" t="s">
+        <v>122</v>
+      </c>
+      <c r="B9" s="87" t="s">
+        <v>122</v>
+      </c>
+      <c r="C9" s="91"/>
+      <c r="D9" s="66" t="s">
+        <v>132</v>
+      </c>
+      <c r="F9" s="96"/>
+      <c r="G9">
+        <v>8</v>
+      </c>
+      <c r="H9" s="87"/>
+      <c r="I9" s="87"/>
+      <c r="J9" s="91"/>
+      <c r="K9" s="66"/>
+    </row>
+    <row r="10" spans="1:26" ht="13.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="87"/>
+      <c r="B10" s="87" t="s">
+        <v>123</v>
+      </c>
+      <c r="C10" s="87" t="s">
+        <v>123</v>
+      </c>
+      <c r="D10" s="66" t="s">
+        <v>133</v>
+      </c>
+      <c r="F10" s="96"/>
+      <c r="G10">
+        <v>9</v>
+      </c>
+      <c r="H10" s="87"/>
+      <c r="I10" s="87"/>
+      <c r="J10" s="87"/>
+      <c r="K10" s="66"/>
+      <c r="M10" s="108" t="s">
+        <v>160</v>
+      </c>
+      <c r="N10" s="106" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" ht="13.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="87" t="s">
+        <v>94</v>
+      </c>
+      <c r="B11" s="87" t="s">
+        <v>94</v>
+      </c>
+      <c r="C11" s="87" t="s">
+        <v>94</v>
+      </c>
+      <c r="D11" s="66" t="s">
+        <v>133</v>
+      </c>
+      <c r="F11" s="96"/>
+      <c r="G11">
+        <v>10</v>
+      </c>
+      <c r="H11" s="87"/>
+      <c r="I11" s="87"/>
+      <c r="J11" s="87"/>
+      <c r="K11" s="66"/>
+      <c r="M11" s="100" t="s">
+        <v>115</v>
+      </c>
+      <c r="N11" s="107"/>
+    </row>
+    <row r="12" spans="1:26" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="87" t="s">
+        <v>95</v>
+      </c>
+      <c r="B12" s="87" t="s">
+        <v>95</v>
+      </c>
+      <c r="C12" s="87" t="s">
+        <v>95</v>
+      </c>
+      <c r="D12" s="66" t="s">
+        <v>133</v>
+      </c>
+      <c r="F12" s="96"/>
+      <c r="G12">
+        <v>11</v>
+      </c>
+      <c r="H12" s="87"/>
+      <c r="I12" s="87"/>
+      <c r="J12" s="87"/>
+      <c r="K12" s="66"/>
+      <c r="S12" s="135"/>
+      <c r="T12" s="135"/>
+      <c r="U12" s="135"/>
+      <c r="V12" s="136"/>
+      <c r="W12" s="137"/>
+      <c r="X12" s="114"/>
+    </row>
+    <row r="13" spans="1:26" ht="13.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="87"/>
+      <c r="B13" s="87" t="s">
+        <v>96</v>
+      </c>
+      <c r="C13" s="87" t="s">
+        <v>96</v>
+      </c>
+      <c r="D13" s="66" t="s">
+        <v>133</v>
+      </c>
+      <c r="F13" s="96"/>
+      <c r="G13">
+        <v>12</v>
+      </c>
+      <c r="H13" s="87"/>
+      <c r="I13" s="87"/>
+      <c r="J13" s="87"/>
+      <c r="K13" s="66"/>
+      <c r="S13" s="138"/>
+      <c r="T13" s="138"/>
+      <c r="U13" s="138"/>
+      <c r="V13" s="114"/>
+      <c r="W13" s="137"/>
+      <c r="X13" s="114"/>
+    </row>
+    <row r="14" spans="1:26" ht="13.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="87" t="s">
+        <v>97</v>
+      </c>
+      <c r="B14" s="87" t="s">
+        <v>97</v>
+      </c>
+      <c r="C14" s="87" t="s">
+        <v>97</v>
+      </c>
+      <c r="D14" s="66" t="s">
+        <v>133</v>
+      </c>
+      <c r="F14" s="96"/>
+      <c r="G14">
+        <v>13</v>
+      </c>
+      <c r="H14" s="87"/>
+      <c r="I14" s="87"/>
+      <c r="J14" s="87"/>
+      <c r="K14" s="66"/>
+      <c r="N14" s="139" t="s">
+        <v>177</v>
+      </c>
+      <c r="O14" s="140"/>
+      <c r="P14" s="140"/>
+      <c r="Q14" s="140"/>
+      <c r="R14" s="140"/>
+      <c r="S14" s="140"/>
+      <c r="T14" s="140"/>
+      <c r="U14" s="141"/>
+      <c r="X14" s="142" t="s">
+        <v>176</v>
+      </c>
+      <c r="Y14" s="143"/>
+      <c r="Z14" s="144"/>
+    </row>
+    <row r="15" spans="1:26" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="87"/>
+      <c r="B15" s="87" t="s">
+        <v>98</v>
+      </c>
+      <c r="C15" s="87" t="s">
+        <v>98</v>
+      </c>
+      <c r="D15" s="66" t="s">
+        <v>133</v>
+      </c>
+      <c r="F15" s="96"/>
+      <c r="G15">
+        <v>14</v>
+      </c>
+      <c r="H15" s="87"/>
+      <c r="I15" s="87"/>
+      <c r="J15" s="87"/>
+      <c r="K15" s="66"/>
+      <c r="S15" t="s">
+        <v>179</v>
+      </c>
+      <c r="T15" t="s">
+        <v>179</v>
+      </c>
+      <c r="U15" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="87" t="s">
+        <v>99</v>
+      </c>
+      <c r="B16" s="87"/>
+      <c r="C16" s="91"/>
+      <c r="D16" s="66" t="s">
+        <v>133</v>
+      </c>
+      <c r="F16" s="96"/>
+      <c r="G16">
+        <v>15</v>
+      </c>
+      <c r="H16" s="87"/>
+      <c r="I16" s="87"/>
+      <c r="J16" s="91"/>
+      <c r="K16" s="66"/>
+      <c r="S16">
+        <f>COUNTA(S20:S39)</f>
+        <v>1</v>
+      </c>
+      <c r="T16">
+        <f>COUNTA(T20:T39)</f>
+        <v>0</v>
+      </c>
+      <c r="U16">
+        <f>COUNTA(U20:U39)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:26" ht="13.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="87" t="s">
+        <v>100</v>
+      </c>
+      <c r="B17" s="87"/>
+      <c r="C17" s="91"/>
+      <c r="D17" s="66" t="s">
+        <v>133</v>
+      </c>
+      <c r="F17" s="96"/>
+      <c r="G17">
+        <v>16</v>
+      </c>
+      <c r="H17" s="87"/>
+      <c r="I17" s="87"/>
+      <c r="J17" s="91"/>
+      <c r="K17" s="66"/>
+    </row>
+    <row r="18" spans="1:26" ht="13.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="87" t="s">
+        <v>101</v>
+      </c>
+      <c r="B18" s="87" t="s">
+        <v>101</v>
+      </c>
+      <c r="C18" s="87" t="s">
+        <v>101</v>
+      </c>
+      <c r="D18" s="66" t="s">
+        <v>133</v>
+      </c>
+      <c r="F18" s="96"/>
+      <c r="G18">
+        <v>17</v>
+      </c>
+      <c r="H18" s="87"/>
+      <c r="I18" s="87"/>
+      <c r="J18" s="87"/>
+      <c r="K18" s="66"/>
+      <c r="N18" s="152" t="s">
+        <v>164</v>
+      </c>
+      <c r="O18" s="153"/>
+      <c r="P18" s="122"/>
+      <c r="Q18" s="145"/>
+      <c r="S18" s="154" t="str">
+        <f>CONCATENATE(S15," ",S16)</f>
+        <v>Numar voturi: 1</v>
+      </c>
+      <c r="T18" s="154" t="str">
+        <f t="shared" ref="T18:U18" si="0">CONCATENATE(T15," ",T16)</f>
+        <v>Numar voturi: 0</v>
+      </c>
+      <c r="U18" s="155" t="str">
+        <f t="shared" si="0"/>
+        <v>Numar voturi: 0</v>
+      </c>
+      <c r="X18" s="132" t="s">
+        <v>174</v>
+      </c>
+      <c r="Y18" s="133" t="s">
+        <v>173</v>
+      </c>
+      <c r="Z18" s="134" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="19" spans="1:26" ht="13.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="87" t="s">
+        <v>102</v>
+      </c>
+      <c r="B19" s="87" t="s">
+        <v>102</v>
+      </c>
+      <c r="C19" s="87" t="s">
+        <v>102</v>
+      </c>
+      <c r="D19" s="66" t="s">
+        <v>133</v>
+      </c>
+      <c r="F19" s="96"/>
+      <c r="G19">
+        <v>18</v>
+      </c>
+      <c r="H19" s="87"/>
+      <c r="I19" s="87"/>
+      <c r="J19" s="87"/>
+      <c r="K19" s="66"/>
+      <c r="N19" s="125" t="s">
+        <v>165</v>
+      </c>
+      <c r="O19" s="126">
+        <v>30</v>
+      </c>
+      <c r="P19" s="88"/>
+      <c r="Q19" s="148"/>
+      <c r="S19" s="119" t="str">
+        <f>O20</f>
+        <v>15-18 Jun</v>
+      </c>
+      <c r="T19" s="119" t="str">
+        <f>O28</f>
+        <v>20-23 Jun</v>
+      </c>
+      <c r="U19" s="119" t="s">
+        <v>167</v>
+      </c>
+      <c r="X19" s="119" t="s">
+        <v>166</v>
+      </c>
+      <c r="Y19" s="119" t="s">
+        <v>167</v>
+      </c>
+      <c r="Z19" s="119" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="20" spans="1:26" ht="13.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="87"/>
+      <c r="B20" s="87" t="s">
+        <v>103</v>
+      </c>
+      <c r="C20" s="91"/>
+      <c r="D20" s="66" t="s">
+        <v>133</v>
+      </c>
+      <c r="F20" s="96"/>
+      <c r="G20">
+        <v>19</v>
+      </c>
+      <c r="H20" s="87"/>
+      <c r="I20" s="87"/>
+      <c r="J20" s="91"/>
+      <c r="K20" s="66"/>
+      <c r="N20" s="117" t="s">
+        <v>168</v>
+      </c>
+      <c r="O20" s="127" t="s">
+        <v>178</v>
+      </c>
+      <c r="P20" s="115"/>
+      <c r="Q20" s="149"/>
+      <c r="S20" s="118" t="str">
+        <f>X20</f>
+        <v>Popescu Alexandru</v>
+      </c>
+      <c r="T20" s="118"/>
+      <c r="U20" s="118"/>
+      <c r="X20" s="118" t="s">
+        <v>175</v>
+      </c>
+      <c r="Y20" s="118"/>
+      <c r="Z20" s="118"/>
+    </row>
+    <row r="21" spans="1:26" ht="13.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="87"/>
+      <c r="B21" s="87" t="s">
+        <v>104</v>
+      </c>
+      <c r="C21" s="91"/>
+      <c r="D21" s="66" t="s">
+        <v>133</v>
+      </c>
+      <c r="F21" s="96"/>
+      <c r="G21">
+        <v>20</v>
+      </c>
+      <c r="H21" s="87"/>
+      <c r="I21" s="87"/>
+      <c r="J21" s="91"/>
+      <c r="K21" s="66"/>
+      <c r="N21" s="120" t="s">
+        <v>158</v>
+      </c>
+      <c r="O21" s="121"/>
+      <c r="S21" s="118"/>
+      <c r="T21" s="118"/>
+      <c r="U21" s="118"/>
+      <c r="X21" s="118"/>
+      <c r="Y21" s="118"/>
+      <c r="Z21" s="118"/>
+    </row>
+    <row r="22" spans="1:26" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="87" t="s">
+        <v>105</v>
+      </c>
+      <c r="B22" s="87" t="s">
+        <v>105</v>
+      </c>
+      <c r="C22" s="87" t="s">
+        <v>105</v>
+      </c>
+      <c r="D22" s="66" t="s">
+        <v>133</v>
+      </c>
+      <c r="F22" s="96"/>
+      <c r="G22">
+        <v>21</v>
+      </c>
+      <c r="H22" s="87"/>
+      <c r="I22" s="87"/>
+      <c r="J22" s="87"/>
+      <c r="K22" s="66"/>
+      <c r="S22" s="118"/>
+      <c r="T22" s="118"/>
+      <c r="U22" s="118"/>
+      <c r="X22" s="118"/>
+      <c r="Y22" s="118"/>
+      <c r="Z22" s="118"/>
+    </row>
+    <row r="23" spans="1:26" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="87" t="s">
+        <v>106</v>
+      </c>
+      <c r="B23" s="87"/>
+      <c r="C23" s="87" t="s">
+        <v>106</v>
+      </c>
+      <c r="D23" s="66" t="s">
+        <v>132</v>
+      </c>
+      <c r="F23" s="96"/>
+      <c r="G23">
+        <v>22</v>
+      </c>
+      <c r="H23" s="87"/>
+      <c r="I23" s="87"/>
+      <c r="J23" s="87"/>
+      <c r="K23" s="66"/>
+      <c r="S23" s="118"/>
+      <c r="T23" s="118"/>
+      <c r="U23" s="118"/>
+      <c r="X23" s="118"/>
+      <c r="Y23" s="118"/>
+      <c r="Z23" s="118"/>
+    </row>
+    <row r="24" spans="1:26" ht="13.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="87"/>
+      <c r="B24" s="87"/>
+      <c r="C24" s="87" t="s">
+        <v>107</v>
+      </c>
+      <c r="D24" s="66" t="s">
+        <v>133</v>
+      </c>
+      <c r="F24" s="96"/>
+      <c r="G24">
+        <v>23</v>
+      </c>
+      <c r="H24" s="87"/>
+      <c r="I24" s="87"/>
+      <c r="J24" s="87"/>
+      <c r="K24" s="66"/>
+      <c r="N24" s="123"/>
+      <c r="O24" s="123"/>
+      <c r="P24" s="123"/>
+      <c r="Q24" s="123"/>
+      <c r="S24" s="118"/>
+      <c r="T24" s="118"/>
+      <c r="U24" s="118"/>
+      <c r="X24" s="118"/>
+      <c r="Y24" s="118"/>
+      <c r="Z24" s="118"/>
+    </row>
+    <row r="25" spans="1:26" ht="13.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="87" t="s">
+        <v>108</v>
+      </c>
+      <c r="B25" s="87" t="s">
+        <v>108</v>
+      </c>
+      <c r="C25" s="87" t="s">
+        <v>108</v>
+      </c>
+      <c r="D25" s="66" t="s">
+        <v>133</v>
+      </c>
+      <c r="F25" s="96"/>
+      <c r="G25">
+        <v>24</v>
+      </c>
+      <c r="H25" s="87"/>
+      <c r="I25" s="87"/>
+      <c r="J25" s="87"/>
+      <c r="K25" s="66"/>
+      <c r="N25" s="152" t="s">
+        <v>164</v>
+      </c>
+      <c r="O25" s="153"/>
+      <c r="P25" s="114"/>
+      <c r="Q25" s="150"/>
+      <c r="S25" s="118"/>
+      <c r="T25" s="118"/>
+      <c r="U25" s="118"/>
+      <c r="X25" s="118"/>
+      <c r="Y25" s="118"/>
+      <c r="Z25" s="118"/>
+    </row>
+    <row r="26" spans="1:26" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="87" t="s">
+        <v>109</v>
+      </c>
+      <c r="B26" s="87" t="s">
+        <v>109</v>
+      </c>
+      <c r="C26" s="87" t="s">
+        <v>109</v>
+      </c>
+      <c r="D26" s="66" t="s">
+        <v>133</v>
+      </c>
+      <c r="F26" s="96"/>
+      <c r="G26">
+        <v>25</v>
+      </c>
+      <c r="H26" s="87"/>
+      <c r="I26" s="87"/>
+      <c r="J26" s="87"/>
+      <c r="K26" s="66"/>
+      <c r="N26" s="125" t="s">
+        <v>165</v>
+      </c>
+      <c r="O26" s="126">
+        <v>30</v>
+      </c>
+      <c r="P26" s="114"/>
+      <c r="Q26" s="151"/>
+      <c r="S26" s="118"/>
+      <c r="T26" s="118"/>
+      <c r="U26" s="118"/>
+      <c r="X26" s="118"/>
+      <c r="Y26" s="118"/>
+      <c r="Z26" s="118"/>
+    </row>
+    <row r="27" spans="1:26" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="87" t="s">
+        <v>110</v>
+      </c>
+      <c r="B27" s="87" t="s">
+        <v>110</v>
+      </c>
+      <c r="C27" s="87" t="s">
+        <v>110</v>
+      </c>
+      <c r="D27" s="66" t="s">
+        <v>133</v>
+      </c>
+      <c r="F27" s="96"/>
+      <c r="G27">
+        <v>26</v>
+      </c>
+      <c r="H27" s="87"/>
+      <c r="I27" s="87"/>
+      <c r="J27" s="87"/>
+      <c r="K27" s="66"/>
+      <c r="N27" s="116" t="s">
+        <v>168</v>
+      </c>
+      <c r="O27" s="130" t="s">
+        <v>178</v>
+      </c>
+      <c r="P27" s="114"/>
+      <c r="Q27" s="148"/>
+      <c r="S27" s="118"/>
+      <c r="T27" s="118"/>
+      <c r="U27" s="118"/>
+      <c r="X27" s="118"/>
+      <c r="Y27" s="118"/>
+      <c r="Z27" s="118"/>
+    </row>
+    <row r="28" spans="1:26" ht="13.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="87" t="s">
+        <v>111</v>
+      </c>
+      <c r="B28" s="87" t="s">
+        <v>111</v>
+      </c>
+      <c r="C28" s="91"/>
+      <c r="D28" s="66" t="s">
+        <v>133</v>
+      </c>
+      <c r="F28" s="96"/>
+      <c r="G28">
+        <v>27</v>
+      </c>
+      <c r="H28" s="87"/>
+      <c r="I28" s="87"/>
+      <c r="J28" s="91"/>
+      <c r="K28" s="66"/>
+      <c r="N28" s="117" t="s">
+        <v>169</v>
+      </c>
+      <c r="O28" s="127" t="s">
+        <v>167</v>
+      </c>
+      <c r="P28" s="114"/>
+      <c r="Q28" s="149"/>
+      <c r="S28" s="118"/>
+      <c r="T28" s="118"/>
+      <c r="U28" s="118"/>
+      <c r="X28" s="118"/>
+      <c r="Y28" s="118"/>
+      <c r="Z28" s="118"/>
+    </row>
+    <row r="29" spans="1:26" ht="13.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="87" t="s">
+        <v>112</v>
+      </c>
+      <c r="B29" s="87" t="s">
+        <v>112</v>
+      </c>
+      <c r="C29" s="87" t="s">
+        <v>112</v>
+      </c>
+      <c r="D29" s="66" t="s">
+        <v>133</v>
+      </c>
+      <c r="F29" s="96"/>
+      <c r="G29">
+        <v>28</v>
+      </c>
+      <c r="H29" s="87"/>
+      <c r="I29" s="87"/>
+      <c r="J29" s="87"/>
+      <c r="K29" s="66"/>
+      <c r="N29" s="128" t="s">
+        <v>158</v>
+      </c>
+      <c r="O29" s="129"/>
+      <c r="P29" s="114"/>
+      <c r="Q29" s="114"/>
+      <c r="S29" s="118"/>
+      <c r="T29" s="118"/>
+      <c r="U29" s="118"/>
+      <c r="X29" s="118"/>
+      <c r="Y29" s="118"/>
+      <c r="Z29" s="118"/>
+    </row>
+    <row r="30" spans="1:26" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="87"/>
+      <c r="B30" s="87" t="s">
+        <v>113</v>
+      </c>
+      <c r="C30" s="87" t="s">
+        <v>113</v>
+      </c>
+      <c r="D30" s="66" t="s">
+        <v>133</v>
+      </c>
+      <c r="F30" s="96"/>
+      <c r="G30">
+        <v>29</v>
+      </c>
+      <c r="H30" s="87"/>
+      <c r="I30" s="87"/>
+      <c r="J30" s="87"/>
+      <c r="K30" s="66"/>
+      <c r="N30" s="137"/>
+      <c r="O30" s="137"/>
+      <c r="P30" s="123"/>
+      <c r="Q30" s="123"/>
+      <c r="S30" s="118"/>
+      <c r="T30" s="118"/>
+      <c r="U30" s="118"/>
+      <c r="X30" s="118"/>
+      <c r="Y30" s="118"/>
+      <c r="Z30" s="118"/>
+    </row>
+    <row r="31" spans="1:26" ht="13.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="87" t="s">
+        <v>114</v>
+      </c>
+      <c r="B31" s="87" t="s">
+        <v>114</v>
+      </c>
+      <c r="C31" s="87" t="s">
+        <v>114</v>
+      </c>
+      <c r="D31" s="66" t="s">
+        <v>133</v>
+      </c>
+      <c r="F31" s="96"/>
+      <c r="G31">
+        <v>30</v>
+      </c>
+      <c r="H31" s="92"/>
+      <c r="I31" s="92"/>
+      <c r="J31" s="92"/>
+      <c r="K31" s="66"/>
+      <c r="N31" s="146"/>
+      <c r="O31" s="138"/>
+      <c r="P31" s="114"/>
+      <c r="Q31" s="124"/>
+      <c r="S31" s="118"/>
+      <c r="T31" s="118"/>
+      <c r="U31" s="118"/>
+      <c r="X31" s="118"/>
+      <c r="Y31" s="118"/>
+      <c r="Z31" s="118"/>
+    </row>
+    <row r="32" spans="1:26" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="94">
+        <f>COUNTA(A2:A31)</f>
+        <v>22</v>
+      </c>
+      <c r="B32" s="94">
+        <f>COUNTA(B2:B31)</f>
+        <v>23</v>
+      </c>
+      <c r="C32" s="94">
+        <f>COUNTA(C2:C31)</f>
+        <v>21</v>
+      </c>
+      <c r="F32" s="96"/>
+      <c r="H32" s="111">
+        <v>14</v>
+      </c>
+      <c r="I32" s="112">
+        <v>24</v>
+      </c>
+      <c r="J32" s="113">
+        <v>5</v>
+      </c>
+      <c r="N32" s="146"/>
+      <c r="O32" s="138"/>
+      <c r="P32" s="114"/>
+      <c r="Q32" s="124"/>
+      <c r="S32" s="118"/>
+      <c r="T32" s="118"/>
+      <c r="U32" s="118"/>
+      <c r="X32" s="118"/>
+      <c r="Y32" s="118"/>
+      <c r="Z32" s="118"/>
+    </row>
+    <row r="33" spans="1:26" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="93"/>
+      <c r="B33" s="93"/>
+      <c r="C33" s="93"/>
+      <c r="F33" s="97"/>
+      <c r="N33" s="146"/>
+      <c r="O33" s="138"/>
+      <c r="P33" s="114"/>
+      <c r="Q33" s="124"/>
+      <c r="S33" s="118"/>
+      <c r="T33" s="118"/>
+      <c r="U33" s="118"/>
+      <c r="X33" s="118"/>
+      <c r="Y33" s="118"/>
+      <c r="Z33" s="118"/>
+    </row>
+    <row r="34" spans="1:26" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="93"/>
+      <c r="B34" s="93"/>
+      <c r="C34" s="93"/>
+      <c r="F34" s="97"/>
+      <c r="N34" s="146"/>
+      <c r="O34" s="138"/>
+      <c r="P34" s="114"/>
+      <c r="Q34" s="124"/>
+      <c r="S34" s="118"/>
+      <c r="T34" s="118"/>
+      <c r="U34" s="118"/>
+      <c r="X34" s="118"/>
+      <c r="Y34" s="118"/>
+      <c r="Z34" s="118"/>
+    </row>
+    <row r="35" spans="1:26" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="93"/>
+      <c r="B35" s="93"/>
+      <c r="C35" s="93"/>
+      <c r="F35" s="97"/>
+      <c r="N35" s="147"/>
+      <c r="O35" s="147"/>
+      <c r="P35" s="114"/>
+      <c r="Q35" s="114"/>
+      <c r="S35" s="118"/>
+      <c r="T35" s="118"/>
+      <c r="U35" s="118"/>
+      <c r="X35" s="118"/>
+      <c r="Y35" s="118"/>
+      <c r="Z35" s="118"/>
+    </row>
+    <row r="36" spans="1:26" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="93"/>
+      <c r="B36" s="93"/>
+      <c r="C36" s="93"/>
+      <c r="F36" s="97"/>
+      <c r="N36" s="114"/>
+      <c r="O36" s="114"/>
+      <c r="P36" s="114"/>
+      <c r="Q36" s="114"/>
+      <c r="S36" s="118"/>
+      <c r="T36" s="118"/>
+      <c r="U36" s="118"/>
+      <c r="X36" s="118"/>
+      <c r="Y36" s="118"/>
+      <c r="Z36" s="118"/>
+    </row>
+    <row r="37" spans="1:26" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="93"/>
+      <c r="B37" s="93"/>
+      <c r="C37" s="93"/>
+      <c r="F37" s="97"/>
+      <c r="N37" s="114"/>
+      <c r="O37" s="114"/>
+      <c r="P37" s="114"/>
+      <c r="Q37" s="114"/>
+      <c r="S37" s="118"/>
+      <c r="T37" s="118"/>
+      <c r="U37" s="118"/>
+      <c r="X37" s="118"/>
+      <c r="Y37" s="118"/>
+      <c r="Z37" s="118"/>
+    </row>
+    <row r="38" spans="1:26" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="93"/>
+      <c r="B38" s="93"/>
+      <c r="C38" s="93"/>
+      <c r="F38" s="97"/>
+      <c r="N38" s="114"/>
+      <c r="O38" s="114"/>
+      <c r="P38" s="114"/>
+      <c r="Q38" s="114"/>
+      <c r="S38" s="118"/>
+      <c r="T38" s="118"/>
+      <c r="U38" s="118"/>
+      <c r="X38" s="118"/>
+      <c r="Y38" s="118"/>
+      <c r="Z38" s="118"/>
+    </row>
+    <row r="39" spans="1:26" ht="13.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="93"/>
+      <c r="B39" s="93"/>
+      <c r="C39" s="93"/>
+      <c r="F39" s="97"/>
+      <c r="S39" s="109"/>
+      <c r="T39" s="109"/>
+      <c r="U39" s="109"/>
+      <c r="X39" s="109"/>
+      <c r="Y39" s="109"/>
+      <c r="Z39" s="109"/>
+    </row>
+    <row r="40" spans="1:26" ht="13.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="93"/>
+      <c r="B40" s="93"/>
+      <c r="C40" s="93"/>
+      <c r="F40" s="98"/>
+    </row>
+    <row r="41" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A41" s="93"/>
+      <c r="B41" s="93"/>
+      <c r="C41" s="93"/>
+    </row>
+    <row r="42" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A42" s="88"/>
+      <c r="B42" s="88"/>
+      <c r="C42" s="88"/>
+    </row>
+  </sheetData>
+  <mergeCells count="13">
+    <mergeCell ref="X14:Z14"/>
+    <mergeCell ref="N14:U14"/>
+    <mergeCell ref="N21:O21"/>
+    <mergeCell ref="N18:O18"/>
+    <mergeCell ref="N35:O35"/>
+    <mergeCell ref="N30:O30"/>
+    <mergeCell ref="R4:R5"/>
+    <mergeCell ref="W12:W13"/>
+    <mergeCell ref="N29:O29"/>
+    <mergeCell ref="N25:O25"/>
+    <mergeCell ref="F1:F32"/>
+    <mergeCell ref="Q1:Q2"/>
+    <mergeCell ref="N10:N11"/>
+  </mergeCells>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D31 K2:K31" xr:uid="{1F392BBB-3D26-4E11-85DF-A7DEBCE7ECA5}">
+      <formula1>$G$2:$G$3</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{A694C1C5-3967-4961-B3CD-322605D6E5F6}">
+          <x14:formula1>
+            <xm:f>'Participation List'!$J$2:$J$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>P2 P5 V13</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D29C6C0-1AA5-4518-814D-180997663027}">
+  <dimension ref="A1:O32"/>
+  <sheetViews>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="0" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="21.5546875" customWidth="1"/>
+    <col min="4" max="4" width="6.21875" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.5546875" customWidth="1"/>
+    <col min="9" max="9" width="8.88671875" customWidth="1"/>
+    <col min="10" max="10" width="15.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B1" s="81" t="s">
         <v>55</v>
       </c>
-      <c r="B1" s="81"/>
-      <c r="C1" s="81"/>
-      <c r="D1" s="81"/>
+      <c r="C1" s="82"/>
+      <c r="D1" s="82"/>
       <c r="E1" s="82"/>
-      <c r="G1" s="61" t="s">
+      <c r="F1" s="83"/>
+      <c r="H1" s="61" t="s">
         <v>61</v>
       </c>
-      <c r="H1" s="61" t="s">
+      <c r="I1" s="61" t="s">
         <v>84</v>
       </c>
-      <c r="I1" s="61" t="s">
+      <c r="J1" s="61" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="79" t="s">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" s="68" t="s">
+        <v>142</v>
+      </c>
+      <c r="B2" s="80" t="s">
         <v>54</v>
       </c>
-      <c r="B2" s="79"/>
-      <c r="C2" s="66" t="s">
+      <c r="C2" s="80"/>
+      <c r="D2" s="66" t="s">
         <v>56</v>
       </c>
-      <c r="D2" s="66" t="s">
+      <c r="E2" s="66" t="s">
         <v>57</v>
       </c>
-      <c r="E2" s="66" t="s">
+      <c r="F2" s="66" t="s">
         <v>2</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>86</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>85</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="78" t="s">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" s="76" t="str">
+        <f>DateVoting!$F$1</f>
+        <v>15-18 Jun</v>
+      </c>
+      <c r="B3" s="79" t="s">
         <v>115</v>
       </c>
-      <c r="B3" s="78"/>
-      <c r="C3" s="66" t="s">
-        <v>86</v>
-      </c>
+      <c r="C3" s="79"/>
       <c r="D3" s="66" t="s">
         <v>86</v>
       </c>
       <c r="E3" s="66" t="s">
+        <v>86</v>
+      </c>
+      <c r="F3" s="66" t="s">
+        <v>132</v>
+      </c>
+      <c r="H3" t="s">
+        <v>58</v>
+      </c>
+      <c r="I3" t="s">
+        <v>86</v>
+      </c>
+      <c r="J3" t="s">
         <v>133</v>
       </c>
-      <c r="G3" t="s">
-        <v>58</v>
-      </c>
-      <c r="H3" t="s">
-        <v>86</v>
-      </c>
-      <c r="I3" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="78" t="s">
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" s="76" t="str">
+        <f>DateVoting!$F$1</f>
+        <v>15-18 Jun</v>
+      </c>
+      <c r="B4" s="79" t="s">
         <v>116</v>
       </c>
-      <c r="B4" s="78"/>
-      <c r="C4" s="66" t="s">
-        <v>86</v>
-      </c>
+      <c r="C4" s="79"/>
       <c r="D4" s="66" t="s">
         <v>86</v>
       </c>
       <c r="E4" s="66" t="s">
+        <v>86</v>
+      </c>
+      <c r="F4" s="66" t="s">
         <v>133</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="78" t="s">
+      <c r="M4" t="s">
+        <v>152</v>
+      </c>
+      <c r="N4" t="s">
+        <v>153</v>
+      </c>
+      <c r="O4" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" s="76" t="str">
+        <f>DateVoting!$F$1</f>
+        <v>15-18 Jun</v>
+      </c>
+      <c r="B5" s="79" t="s">
         <v>117</v>
       </c>
-      <c r="B5" s="78"/>
-      <c r="C5" s="66" t="s">
+      <c r="C5" s="79"/>
+      <c r="D5" s="66" t="s">
         <v>85</v>
       </c>
-      <c r="D5" s="66" t="s">
+      <c r="E5" s="66" t="s">
         <v>58</v>
       </c>
-      <c r="E5" s="66" t="s">
+      <c r="F5" s="66" t="s">
         <v>133</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="78" t="s">
+      <c r="N5" t="s">
+        <v>154</v>
+      </c>
+      <c r="O5" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" s="76" t="str">
+        <f>DateVoting!$F$1</f>
+        <v>15-18 Jun</v>
+      </c>
+      <c r="B6" s="79" t="s">
         <v>118</v>
       </c>
-      <c r="B6" s="78"/>
-      <c r="C6" s="66" t="s">
-        <v>86</v>
-      </c>
+      <c r="C6" s="79"/>
       <c r="D6" s="66" t="s">
         <v>86</v>
       </c>
       <c r="E6" s="66" t="s">
+        <v>86</v>
+      </c>
+      <c r="F6" s="66" t="s">
         <v>132</v>
       </c>
-      <c r="G6" t="s">
+      <c r="H6" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="78" t="s">
+      <c r="N6" t="s">
+        <v>155</v>
+      </c>
+      <c r="O6" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7" s="76" t="str">
+        <f>DateVoting!$F$1</f>
+        <v>15-18 Jun</v>
+      </c>
+      <c r="B7" s="79" t="s">
         <v>119</v>
       </c>
-      <c r="B7" s="78"/>
-      <c r="C7" s="66" t="s">
+      <c r="C7" s="79"/>
+      <c r="D7" s="66" t="s">
         <v>85</v>
       </c>
-      <c r="D7" s="66" t="s">
+      <c r="E7" s="66" t="s">
         <v>86</v>
       </c>
-      <c r="E7" s="66" t="s">
+      <c r="F7" s="66" t="s">
         <v>133</v>
       </c>
-      <c r="G7" t="s">
+      <c r="H7" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="78" t="s">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8" s="76" t="str">
+        <f>DateVoting!$F$1</f>
+        <v>15-18 Jun</v>
+      </c>
+      <c r="B8" s="79" t="s">
         <v>120</v>
       </c>
-      <c r="B8" s="78"/>
-      <c r="C8" s="66" t="s">
+      <c r="C8" s="79"/>
+      <c r="D8" s="66" t="s">
         <v>85</v>
       </c>
-      <c r="D8" s="66" t="s">
+      <c r="E8" s="66" t="s">
         <v>86</v>
       </c>
-      <c r="E8" s="66" t="s">
+      <c r="F8" s="66" t="s">
         <v>133</v>
       </c>
-      <c r="G8" t="s">
+      <c r="H8" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="78" t="s">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9" s="76" t="str">
+        <f>DateVoting!$F$1</f>
+        <v>15-18 Jun</v>
+      </c>
+      <c r="B9" s="79" t="s">
         <v>121</v>
       </c>
-      <c r="B9" s="78"/>
-      <c r="C9" s="66" t="s">
-        <v>86</v>
-      </c>
+      <c r="C9" s="79"/>
       <c r="D9" s="66" t="s">
         <v>86</v>
       </c>
       <c r="E9" s="66" t="s">
+        <v>86</v>
+      </c>
+      <c r="F9" s="66" t="s">
         <v>133</v>
       </c>
-      <c r="G9" t="s">
+      <c r="H9" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="78" t="s">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10" s="76" t="str">
+        <f>DateVoting!$F$1</f>
+        <v>15-18 Jun</v>
+      </c>
+      <c r="B10" s="79" t="s">
         <v>122</v>
       </c>
-      <c r="B10" s="78"/>
-      <c r="C10" s="66" t="s">
+      <c r="C10" s="79"/>
+      <c r="D10" s="66" t="s">
         <v>86</v>
       </c>
-      <c r="D10" s="66" t="s">
+      <c r="E10" s="66" t="s">
         <v>68</v>
       </c>
-      <c r="E10" s="66" t="s">
+      <c r="F10" s="66" t="s">
         <v>132</v>
       </c>
-      <c r="G10" t="s">
+      <c r="H10" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="78" t="s">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A11" s="76" t="str">
+        <f>DateVoting!$F$1</f>
+        <v>15-18 Jun</v>
+      </c>
+      <c r="B11" s="79" t="s">
         <v>123</v>
       </c>
-      <c r="B11" s="78"/>
-      <c r="C11" s="66" t="s">
-        <v>86</v>
-      </c>
+      <c r="C11" s="79"/>
       <c r="D11" s="66" t="s">
         <v>86</v>
       </c>
       <c r="E11" s="66" t="s">
+        <v>86</v>
+      </c>
+      <c r="F11" s="66" t="s">
         <v>133</v>
       </c>
-      <c r="G11" t="s">
+      <c r="H11" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="78" t="s">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A12" s="76" t="str">
+        <f>DateVoting!$F$1</f>
+        <v>15-18 Jun</v>
+      </c>
+      <c r="B12" s="79" t="s">
         <v>94</v>
       </c>
-      <c r="B12" s="78"/>
-      <c r="C12" s="66" t="s">
+      <c r="C12" s="79"/>
+      <c r="D12" s="66" t="s">
         <v>85</v>
       </c>
-      <c r="D12" s="66" t="s">
+      <c r="E12" s="66" t="s">
         <v>86</v>
       </c>
-      <c r="E12" s="66" t="s">
+      <c r="F12" s="66" t="s">
         <v>133</v>
       </c>
-      <c r="G12" t="s">
+      <c r="H12" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="78" t="s">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A13" s="76" t="str">
+        <f>DateVoting!$F$1</f>
+        <v>15-18 Jun</v>
+      </c>
+      <c r="B13" s="79" t="s">
         <v>95</v>
       </c>
-      <c r="B13" s="78"/>
-      <c r="C13" s="66" t="s">
-        <v>86</v>
-      </c>
+      <c r="C13" s="79"/>
       <c r="D13" s="66" t="s">
         <v>86</v>
       </c>
       <c r="E13" s="66" t="s">
+        <v>86</v>
+      </c>
+      <c r="F13" s="66" t="s">
         <v>133</v>
       </c>
-      <c r="G13" t="s">
+      <c r="H13" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="78" t="s">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A14" s="76" t="str">
+        <f>DateVoting!$F$1</f>
+        <v>15-18 Jun</v>
+      </c>
+      <c r="B14" s="79" t="s">
         <v>96</v>
       </c>
-      <c r="B14" s="78"/>
-      <c r="C14" s="66" t="s">
-        <v>86</v>
-      </c>
+      <c r="C14" s="79"/>
       <c r="D14" s="66" t="s">
         <v>86</v>
       </c>
       <c r="E14" s="66" t="s">
+        <v>86</v>
+      </c>
+      <c r="F14" s="66" t="s">
         <v>133</v>
       </c>
-      <c r="G14" t="s">
+      <c r="H14" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="78" t="s">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A15" s="76" t="str">
+        <f>DateVoting!$F$1</f>
+        <v>15-18 Jun</v>
+      </c>
+      <c r="B15" s="79" t="s">
         <v>97</v>
       </c>
-      <c r="B15" s="78"/>
-      <c r="C15" s="66" t="s">
-        <v>86</v>
-      </c>
+      <c r="C15" s="79"/>
       <c r="D15" s="66" t="s">
         <v>86</v>
       </c>
       <c r="E15" s="66" t="s">
+        <v>86</v>
+      </c>
+      <c r="F15" s="66" t="s">
         <v>133</v>
       </c>
-      <c r="G15" t="s">
+      <c r="H15" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="78" t="s">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A16" s="76" t="str">
+        <f>DateVoting!$F$1</f>
+        <v>15-18 Jun</v>
+      </c>
+      <c r="B16" s="79" t="s">
         <v>98</v>
       </c>
-      <c r="B16" s="78"/>
-      <c r="C16" s="66" t="s">
+      <c r="C16" s="79"/>
+      <c r="D16" s="66" t="s">
         <v>85</v>
       </c>
-      <c r="D16" s="66" t="s">
+      <c r="E16" s="66" t="s">
         <v>69</v>
       </c>
-      <c r="E16" s="66" t="s">
+      <c r="F16" s="66" t="s">
         <v>133</v>
       </c>
-      <c r="G16" t="s">
+      <c r="H16" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="78" t="s">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="76" t="str">
+        <f>DateVoting!$F$1</f>
+        <v>15-18 Jun</v>
+      </c>
+      <c r="B17" s="79" t="s">
         <v>99</v>
       </c>
-      <c r="B17" s="78"/>
-      <c r="C17" s="66" t="s">
+      <c r="C17" s="79"/>
+      <c r="D17" s="66" t="s">
         <v>85</v>
       </c>
-      <c r="D17" s="66" t="s">
+      <c r="E17" s="66" t="s">
         <v>64</v>
       </c>
-      <c r="E17" s="66" t="s">
+      <c r="F17" s="66" t="s">
         <v>133</v>
       </c>
-      <c r="G17" t="s">
+      <c r="H17" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="78" t="s">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="76" t="str">
+        <f>DateVoting!$F$1</f>
+        <v>15-18 Jun</v>
+      </c>
+      <c r="B18" s="79" t="s">
         <v>100</v>
       </c>
-      <c r="B18" s="78"/>
-      <c r="C18" s="66" t="s">
+      <c r="C18" s="79"/>
+      <c r="D18" s="66" t="s">
         <v>85</v>
       </c>
-      <c r="D18" s="66" t="s">
+      <c r="E18" s="66" t="s">
         <v>86</v>
       </c>
-      <c r="E18" s="66" t="s">
+      <c r="F18" s="66" t="s">
         <v>133</v>
       </c>
-      <c r="G18" t="s">
+      <c r="H18" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="78" t="s">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="76" t="str">
+        <f>DateVoting!$F$1</f>
+        <v>15-18 Jun</v>
+      </c>
+      <c r="B19" s="79" t="s">
         <v>101</v>
       </c>
-      <c r="B19" s="78"/>
-      <c r="C19" s="66" t="s">
-        <v>86</v>
-      </c>
+      <c r="C19" s="79"/>
       <c r="D19" s="66" t="s">
         <v>86</v>
       </c>
       <c r="E19" s="66" t="s">
+        <v>86</v>
+      </c>
+      <c r="F19" s="66" t="s">
         <v>133</v>
       </c>
-      <c r="G19" t="s">
+      <c r="H19" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="78" t="s">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="76" t="str">
+        <f>DateVoting!$F$1</f>
+        <v>15-18 Jun</v>
+      </c>
+      <c r="B20" s="79" t="s">
         <v>102</v>
       </c>
-      <c r="B20" s="78"/>
-      <c r="C20" s="66" t="s">
-        <v>86</v>
-      </c>
+      <c r="C20" s="79"/>
       <c r="D20" s="66" t="s">
         <v>86</v>
       </c>
       <c r="E20" s="66" t="s">
+        <v>86</v>
+      </c>
+      <c r="F20" s="66" t="s">
         <v>133</v>
       </c>
-      <c r="G20" t="s">
+      <c r="H20" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="78" t="s">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="76" t="str">
+        <f>DateVoting!$F$1</f>
+        <v>15-18 Jun</v>
+      </c>
+      <c r="B21" s="79" t="s">
         <v>103</v>
       </c>
-      <c r="B21" s="78"/>
-      <c r="C21" s="66" t="s">
-        <v>86</v>
-      </c>
+      <c r="C21" s="79"/>
       <c r="D21" s="66" t="s">
         <v>86</v>
       </c>
       <c r="E21" s="66" t="s">
+        <v>86</v>
+      </c>
+      <c r="F21" s="66" t="s">
         <v>133</v>
       </c>
-      <c r="G21" t="s">
+      <c r="H21" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="78" t="s">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="76" t="str">
+        <f>DateVoting!$F$1</f>
+        <v>15-18 Jun</v>
+      </c>
+      <c r="B22" s="79" t="s">
         <v>104</v>
       </c>
-      <c r="B22" s="78"/>
-      <c r="C22" s="66" t="s">
-        <v>86</v>
-      </c>
+      <c r="C22" s="79"/>
       <c r="D22" s="66" t="s">
         <v>86</v>
       </c>
       <c r="E22" s="66" t="s">
+        <v>86</v>
+      </c>
+      <c r="F22" s="66" t="s">
         <v>133</v>
       </c>
-      <c r="G22" t="s">
+      <c r="H22" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="78" t="s">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="76" t="str">
+        <f>DateVoting!$F$1</f>
+        <v>15-18 Jun</v>
+      </c>
+      <c r="B23" s="79" t="s">
         <v>105</v>
       </c>
-      <c r="B23" s="78"/>
-      <c r="C23" s="66" t="s">
+      <c r="C23" s="79"/>
+      <c r="D23" s="66" t="s">
         <v>85</v>
       </c>
-      <c r="D23" s="66" t="s">
+      <c r="E23" s="66" t="s">
         <v>86</v>
       </c>
-      <c r="E23" s="66" t="s">
+      <c r="F23" s="66" t="s">
         <v>133</v>
       </c>
-      <c r="G23" t="s">
+      <c r="H23" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="78" t="s">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="76" t="str">
+        <f>DateVoting!$F$1</f>
+        <v>15-18 Jun</v>
+      </c>
+      <c r="B24" s="79" t="s">
         <v>106</v>
       </c>
-      <c r="B24" s="78"/>
-      <c r="C24" s="66" t="s">
-        <v>86</v>
-      </c>
+      <c r="C24" s="79"/>
       <c r="D24" s="66" t="s">
         <v>86</v>
       </c>
       <c r="E24" s="66" t="s">
+        <v>86</v>
+      </c>
+      <c r="F24" s="66" t="s">
         <v>132</v>
       </c>
-      <c r="G24" t="s">
+      <c r="H24" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="78" t="s">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="76" t="str">
+        <f>DateVoting!$F$1</f>
+        <v>15-18 Jun</v>
+      </c>
+      <c r="B25" s="79" t="s">
         <v>107</v>
       </c>
-      <c r="B25" s="78"/>
-      <c r="C25" s="66" t="s">
-        <v>86</v>
-      </c>
+      <c r="C25" s="79"/>
       <c r="D25" s="66" t="s">
         <v>86</v>
       </c>
       <c r="E25" s="66" t="s">
+        <v>86</v>
+      </c>
+      <c r="F25" s="66" t="s">
         <v>133</v>
       </c>
-      <c r="G25" t="s">
+      <c r="H25" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="78" t="s">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="76" t="str">
+        <f>DateVoting!$F$1</f>
+        <v>15-18 Jun</v>
+      </c>
+      <c r="B26" s="79" t="s">
         <v>108</v>
       </c>
-      <c r="B26" s="78"/>
-      <c r="C26" s="66" t="s">
+      <c r="C26" s="79"/>
+      <c r="D26" s="66" t="s">
         <v>86</v>
       </c>
-      <c r="D26" s="66" t="s">
+      <c r="E26" s="66" t="s">
         <v>58</v>
       </c>
-      <c r="E26" s="66" t="s">
+      <c r="F26" s="66" t="s">
         <v>133</v>
       </c>
-      <c r="G26" t="s">
+      <c r="H26" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="78" t="s">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" s="76" t="str">
+        <f>DateVoting!$F$1</f>
+        <v>15-18 Jun</v>
+      </c>
+      <c r="B27" s="79" t="s">
         <v>109</v>
       </c>
-      <c r="B27" s="78"/>
-      <c r="C27" s="66" t="s">
+      <c r="C27" s="79"/>
+      <c r="D27" s="66" t="s">
         <v>85</v>
       </c>
-      <c r="D27" s="66" t="s">
+      <c r="E27" s="66" t="s">
         <v>86</v>
       </c>
-      <c r="E27" s="66" t="s">
+      <c r="F27" s="66" t="s">
         <v>133</v>
       </c>
-      <c r="G27" t="s">
+      <c r="H27" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="78" t="s">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" s="76" t="str">
+        <f>DateVoting!$F$1</f>
+        <v>15-18 Jun</v>
+      </c>
+      <c r="B28" s="79" t="s">
         <v>110</v>
       </c>
-      <c r="B28" s="78"/>
-      <c r="C28" s="66" t="s">
-        <v>86</v>
-      </c>
+      <c r="C28" s="79"/>
       <c r="D28" s="66" t="s">
         <v>86</v>
       </c>
       <c r="E28" s="66" t="s">
+        <v>86</v>
+      </c>
+      <c r="F28" s="66" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="78" t="s">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" s="76" t="str">
+        <f>DateVoting!$F$1</f>
+        <v>15-18 Jun</v>
+      </c>
+      <c r="B29" s="79" t="s">
         <v>111</v>
       </c>
-      <c r="B29" s="78"/>
-      <c r="C29" s="66" t="s">
-        <v>86</v>
-      </c>
+      <c r="C29" s="79"/>
       <c r="D29" s="66" t="s">
         <v>86</v>
       </c>
       <c r="E29" s="66" t="s">
+        <v>86</v>
+      </c>
+      <c r="F29" s="66" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="78" t="s">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" s="76" t="str">
+        <f>DateVoting!$F$1</f>
+        <v>15-18 Jun</v>
+      </c>
+      <c r="B30" s="79" t="s">
         <v>112</v>
       </c>
-      <c r="B30" s="78"/>
-      <c r="C30" s="66" t="s">
+      <c r="C30" s="79"/>
+      <c r="D30" s="66" t="s">
         <v>85</v>
       </c>
-      <c r="D30" s="66" t="s">
+      <c r="E30" s="66" t="s">
         <v>63</v>
       </c>
-      <c r="E30" s="66" t="s">
+      <c r="F30" s="66" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="78" t="s">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" s="76" t="str">
+        <f>DateVoting!$F$1</f>
+        <v>15-18 Jun</v>
+      </c>
+      <c r="B31" s="79" t="s">
         <v>113</v>
       </c>
-      <c r="B31" s="78"/>
-      <c r="C31" s="66" t="s">
-        <v>86</v>
-      </c>
+      <c r="C31" s="79"/>
       <c r="D31" s="66" t="s">
         <v>86</v>
       </c>
       <c r="E31" s="66" t="s">
+        <v>86</v>
+      </c>
+      <c r="F31" s="66" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="78" t="s">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" s="76" t="str">
+        <f>DateVoting!$F$1</f>
+        <v>15-18 Jun</v>
+      </c>
+      <c r="B32" s="79" t="s">
         <v>114</v>
       </c>
-      <c r="B32" s="78"/>
-      <c r="C32" s="66" t="s">
-        <v>86</v>
-      </c>
+      <c r="C32" s="79"/>
       <c r="D32" s="66" t="s">
         <v>86</v>
       </c>
       <c r="E32" s="66" t="s">
+        <v>86</v>
+      </c>
+      <c r="F32" s="66" t="s">
         <v>133</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="32">
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B10:C10"/>
   </mergeCells>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E32" xr:uid="{AD533C06-5237-486A-8404-42C5B3D58852}">
-      <formula1>$I$2:$I$3</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3:F32" xr:uid="{AD533C06-5237-486A-8404-42C5B3D58852}">
+      <formula1>$J$2:$J$3</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D3:D32" xr:uid="{9FDDCE2D-A2F0-4222-B31F-9AF99710446C}">
-      <formula1>$G$2:$G$27</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E32" xr:uid="{9FDDCE2D-A2F0-4222-B31F-9AF99710446C}">
+      <formula1>$H$2:$H$27</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3:C32" xr:uid="{B64CC271-93F7-4AB1-8CD9-F21CAECF9ACD}">
-      <formula1>IF(#REF!="X", $H$2:$H$3, #REF!)</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D3:D32" xr:uid="{B64CC271-93F7-4AB1-8CD9-F21CAECF9ACD}">
+      <formula1>IF(#REF!="X", $I$2:$I$3, #REF!)</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3395,11 +5346,437 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5F48C49-4C81-44FE-B390-3476598A67D7}">
+  <dimension ref="A3:I34"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I19" sqref="I19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.21875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="76" t="s">
+        <v>144</v>
+      </c>
+      <c r="C3" s="79" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="79"/>
+      <c r="E3" s="86"/>
+      <c r="F3" s="79" t="s">
+        <v>143</v>
+      </c>
+      <c r="G3" s="79"/>
+      <c r="I3" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="64" t="str">
+        <f>DateVoting!F1</f>
+        <v>15-18 Jun</v>
+      </c>
+      <c r="B4" s="62"/>
+      <c r="C4" s="64" t="s">
+        <v>145</v>
+      </c>
+      <c r="D4" s="64" t="s">
+        <v>146</v>
+      </c>
+      <c r="E4" s="62"/>
+      <c r="F4" s="64" t="s">
+        <v>147</v>
+      </c>
+      <c r="G4" s="64" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="87">
+        <f>DateVoting!B2</f>
+        <v>0</v>
+      </c>
+      <c r="C5" s="87" t="s">
+        <v>115</v>
+      </c>
+      <c r="D5" s="87" t="s">
+        <v>118</v>
+      </c>
+      <c r="E5" s="87"/>
+      <c r="F5" s="66"/>
+      <c r="G5" s="66"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="87" t="str">
+        <f>DateVoting!B3</f>
+        <v>Andreea Ionescu</v>
+      </c>
+      <c r="C6" s="87" t="s">
+        <v>116</v>
+      </c>
+      <c r="D6" s="87" t="s">
+        <v>122</v>
+      </c>
+      <c r="E6" s="87"/>
+      <c r="F6" s="66"/>
+      <c r="G6" s="66"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="87">
+        <f>DateVoting!B4</f>
+        <v>0</v>
+      </c>
+      <c r="C7" s="87" t="s">
+        <v>117</v>
+      </c>
+      <c r="D7" s="87" t="s">
+        <v>106</v>
+      </c>
+      <c r="E7" s="87"/>
+      <c r="F7" s="66"/>
+      <c r="G7" s="66"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="87" t="str">
+        <f>DateVoting!B5</f>
+        <v>Elena Radu</v>
+      </c>
+      <c r="C8" s="87" t="s">
+        <v>119</v>
+      </c>
+      <c r="D8" s="87"/>
+      <c r="F8" s="66"/>
+      <c r="G8" s="66"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="87">
+        <f>DateVoting!B6</f>
+        <v>0</v>
+      </c>
+      <c r="C9" s="87" t="s">
+        <v>120</v>
+      </c>
+      <c r="D9" s="87"/>
+      <c r="F9" s="66"/>
+      <c r="G9" s="66"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="87" t="str">
+        <f>DateVoting!B7</f>
+        <v>Gabriela Dima</v>
+      </c>
+      <c r="C10" s="87" t="s">
+        <v>121</v>
+      </c>
+      <c r="D10" s="87"/>
+      <c r="F10" s="66"/>
+      <c r="G10" s="66"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="87" t="str">
+        <f>DateVoting!B8</f>
+        <v>Adrian Mihai</v>
+      </c>
+      <c r="C11" s="87" t="s">
+        <v>123</v>
+      </c>
+      <c r="D11" s="87"/>
+      <c r="F11" s="66"/>
+      <c r="G11" s="66"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="87" t="str">
+        <f>DateVoting!B9</f>
+        <v>Laura Tudor</v>
+      </c>
+      <c r="C12" s="87" t="s">
+        <v>94</v>
+      </c>
+      <c r="D12" s="87"/>
+      <c r="F12" s="66"/>
+      <c r="G12" s="66"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="87" t="str">
+        <f>DateVoting!B10</f>
+        <v>Andrei Nistor</v>
+      </c>
+      <c r="C13" s="87" t="s">
+        <v>95</v>
+      </c>
+      <c r="D13" s="87"/>
+      <c r="F13" s="66"/>
+      <c r="G13" s="66"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="87" t="str">
+        <f>DateVoting!B11</f>
+        <v>Ana Dumitru</v>
+      </c>
+      <c r="C14" s="87" t="s">
+        <v>96</v>
+      </c>
+      <c r="D14" s="87"/>
+      <c r="F14" s="66"/>
+      <c r="G14" s="66"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="87" t="str">
+        <f>DateVoting!B12</f>
+        <v>Radu Moldovan</v>
+      </c>
+      <c r="C15" s="87" t="s">
+        <v>97</v>
+      </c>
+      <c r="D15" s="87"/>
+      <c r="F15" s="66"/>
+      <c r="G15" s="66"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="87" t="str">
+        <f>DateVoting!B13</f>
+        <v>Ioana Cojocaru</v>
+      </c>
+      <c r="C16" s="87" t="s">
+        <v>98</v>
+      </c>
+      <c r="D16" s="87"/>
+      <c r="F16" s="66"/>
+      <c r="G16" s="66"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="87" t="str">
+        <f>DateVoting!B14</f>
+        <v>Florin Stan</v>
+      </c>
+      <c r="C17" s="87" t="s">
+        <v>99</v>
+      </c>
+      <c r="D17" s="87"/>
+      <c r="F17" s="66"/>
+      <c r="G17" s="66"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="87" t="str">
+        <f>DateVoting!B15</f>
+        <v>Mihaela Popa</v>
+      </c>
+      <c r="C18" s="87" t="s">
+        <v>100</v>
+      </c>
+      <c r="D18" s="87"/>
+      <c r="F18" s="66"/>
+      <c r="G18" s="66"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="87">
+        <f>DateVoting!B16</f>
+        <v>0</v>
+      </c>
+      <c r="C19" s="87" t="s">
+        <v>101</v>
+      </c>
+      <c r="D19" s="87"/>
+      <c r="F19" s="66"/>
+      <c r="G19" s="66"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="87">
+        <f>DateVoting!B17</f>
+        <v>0</v>
+      </c>
+      <c r="C20" s="87" t="s">
+        <v>102</v>
+      </c>
+      <c r="D20" s="87"/>
+      <c r="F20" s="66"/>
+      <c r="G20" s="66"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="87" t="str">
+        <f>DateVoting!B18</f>
+        <v>Sorin Neagu</v>
+      </c>
+      <c r="C21" s="87" t="s">
+        <v>103</v>
+      </c>
+      <c r="D21" s="87"/>
+      <c r="F21" s="66"/>
+      <c r="G21" s="66"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="87" t="str">
+        <f>DateVoting!B19</f>
+        <v>Diana Ionita</v>
+      </c>
+      <c r="C22" s="87" t="s">
+        <v>104</v>
+      </c>
+      <c r="D22" s="87"/>
+      <c r="F22" s="66"/>
+      <c r="G22" s="66"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="87" t="str">
+        <f>DateVoting!B20</f>
+        <v>Victor Luca</v>
+      </c>
+      <c r="C23" s="87" t="s">
+        <v>105</v>
+      </c>
+      <c r="D23" s="87"/>
+      <c r="F23" s="66"/>
+      <c r="G23" s="66"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="87" t="str">
+        <f>DateVoting!B21</f>
+        <v>Roxana Costin</v>
+      </c>
+      <c r="C24" s="87" t="s">
+        <v>107</v>
+      </c>
+      <c r="D24" s="87"/>
+      <c r="F24" s="66"/>
+      <c r="G24" s="66"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="87" t="str">
+        <f>DateVoting!B22</f>
+        <v>Andrei Pop</v>
+      </c>
+      <c r="C25" s="87" t="s">
+        <v>108</v>
+      </c>
+      <c r="D25" s="87"/>
+      <c r="F25" s="66"/>
+      <c r="G25" s="66"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="87">
+        <f>DateVoting!B23</f>
+        <v>0</v>
+      </c>
+      <c r="C26" s="87" t="s">
+        <v>109</v>
+      </c>
+      <c r="D26" s="87"/>
+      <c r="F26" s="66"/>
+      <c r="G26" s="66"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="87">
+        <f>DateVoting!B24</f>
+        <v>0</v>
+      </c>
+      <c r="C27" s="87" t="s">
+        <v>110</v>
+      </c>
+      <c r="D27" s="87"/>
+      <c r="F27" s="66"/>
+      <c r="G27" s="66"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="87" t="str">
+        <f>DateVoting!B25</f>
+        <v>Larisa Constantinescu</v>
+      </c>
+      <c r="C28" s="87" t="s">
+        <v>111</v>
+      </c>
+      <c r="D28" s="87"/>
+      <c r="F28" s="66"/>
+      <c r="G28" s="66"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="87" t="str">
+        <f>DateVoting!B26</f>
+        <v>Bogdan Stoian</v>
+      </c>
+      <c r="C29" s="87" t="s">
+        <v>112</v>
+      </c>
+      <c r="D29" s="87"/>
+      <c r="F29" s="66"/>
+      <c r="G29" s="66"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="87" t="str">
+        <f>DateVoting!B27</f>
+        <v>Carmen Vasile</v>
+      </c>
+      <c r="C30" s="87" t="s">
+        <v>113</v>
+      </c>
+      <c r="D30" s="87"/>
+      <c r="F30" s="66"/>
+      <c r="G30" s="66"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="87" t="str">
+        <f>DateVoting!B28</f>
+        <v>Ciprian Iordache</v>
+      </c>
+      <c r="C31" s="87" t="s">
+        <v>114</v>
+      </c>
+      <c r="D31" s="87"/>
+      <c r="F31" s="66"/>
+      <c r="G31" s="66"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" s="87" t="str">
+        <f>DateVoting!B29</f>
+        <v>Simona Marinescu</v>
+      </c>
+      <c r="C32" s="66"/>
+      <c r="D32" s="66"/>
+      <c r="F32" s="66"/>
+      <c r="G32" s="66"/>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" s="87" t="str">
+        <f>DateVoting!B30</f>
+        <v>Vlad Sandu</v>
+      </c>
+      <c r="C33" s="66"/>
+      <c r="D33" s="66"/>
+      <c r="F33" s="66"/>
+      <c r="G33" s="66"/>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" s="87" t="str">
+        <f>DateVoting!B31</f>
+        <v>Ioana Radulescu</v>
+      </c>
+      <c r="C34" s="66"/>
+      <c r="D34" s="66"/>
+      <c r="F34" s="66"/>
+      <c r="G34" s="66"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="F3:G3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A94A1BE0-93F2-4C18-9D5C-FE2D9F3472AE}">
   <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -3417,40 +5794,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A1" s="83" t="s">
+      <c r="A1" s="84" t="s">
         <v>88</v>
       </c>
-      <c r="B1" s="83"/>
-      <c r="C1" s="83"/>
+      <c r="B1" s="84"/>
+      <c r="C1" s="84"/>
       <c r="D1" s="62"/>
-      <c r="E1" s="83" t="s">
+      <c r="E1" s="84" t="s">
         <v>46</v>
       </c>
-      <c r="F1" s="83"/>
-      <c r="G1" s="83"/>
-      <c r="I1" s="83" t="s">
+      <c r="F1" s="84"/>
+      <c r="G1" s="84"/>
+      <c r="I1" s="84" t="s">
         <v>47</v>
       </c>
-      <c r="J1" s="83"/>
-      <c r="K1" s="83"/>
+      <c r="J1" s="84"/>
+      <c r="K1" s="84"/>
     </row>
     <row r="2" spans="1:11" ht="22.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="84" t="str">
+      <c r="A2" s="85" t="str">
         <f>Location!B2</f>
         <v>Pensiunea Valea Zanelor</v>
       </c>
-      <c r="B2" s="84"/>
-      <c r="C2" s="84"/>
-      <c r="E2" s="84" t="s">
+      <c r="B2" s="85"/>
+      <c r="C2" s="85"/>
+      <c r="E2" s="85" t="s">
         <v>51</v>
       </c>
-      <c r="F2" s="84"/>
-      <c r="G2" s="84"/>
-      <c r="I2" s="84" t="s">
+      <c r="F2" s="85"/>
+      <c r="G2" s="85"/>
+      <c r="I2" s="85" t="s">
         <v>52</v>
       </c>
-      <c r="J2" s="84"/>
-      <c r="K2" s="84"/>
+      <c r="J2" s="85"/>
+      <c r="K2" s="85"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="64" t="s">
@@ -3520,7 +5897,7 @@
         <v>0.5</v>
       </c>
       <c r="C5" s="65">
-        <f>Location!B3</f>
+        <f>Location!B4</f>
         <v>2500</v>
       </c>
       <c r="D5" s="45"/>
@@ -3690,28 +6067,30 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACE780CE-1C58-49A2-9B78-7393F891FAAC}">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A1:B13"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="27.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="82.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A1" s="83" t="s">
+    <row r="1" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.25">
+      <c r="A1" s="84" t="s">
         <v>88</v>
       </c>
-      <c r="B1" s="83"/>
+      <c r="B1" s="84"/>
       <c r="C1" s="70"/>
     </row>
-    <row r="2" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A2" s="66" t="s">
         <v>124</v>
       </c>
@@ -3719,69 +6098,96 @@
         <v>49</v>
       </c>
       <c r="C2" s="69"/>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E2" s="66" t="s">
+        <v>124</v>
+      </c>
+      <c r="F2" s="66" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A3" s="66" t="s">
+        <v>171</v>
+      </c>
+      <c r="B3" s="131" t="s">
+        <v>172</v>
+      </c>
+      <c r="C3" s="69"/>
+      <c r="E3" s="66" t="s">
+        <v>171</v>
+      </c>
+      <c r="F3" s="131" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="66" t="s">
         <v>53</v>
       </c>
-      <c r="B3" s="71">
+      <c r="B4" s="71">
         <v>2500</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="66" t="s">
+      <c r="E4" s="66" t="s">
+        <v>130</v>
+      </c>
+      <c r="F4" s="68" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="66" t="s">
         <v>93</v>
       </c>
-      <c r="B4" s="72">
-        <f>COUNTA('Participation List'!A3:B32)</f>
+      <c r="B5" s="72">
+        <f>COUNTA('Participation List'!B3:C32)</f>
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="66" t="s">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="66" t="s">
         <v>130</v>
       </c>
-      <c r="B5" s="68" t="s">
+      <c r="B6" s="68" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="66" t="s">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="66" t="s">
         <v>87</v>
       </c>
-      <c r="B6" s="73">
+      <c r="B7" s="73">
         <v>300</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="66" t="s">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="66" t="s">
         <v>89</v>
       </c>
-      <c r="B7" s="68" t="s">
+      <c r="B8" s="68" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="66" t="s">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="66" t="s">
         <v>90</v>
-      </c>
-      <c r="B8" s="68" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="66" t="s">
-        <v>91</v>
       </c>
       <c r="B9" s="68" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="66" t="s">
+        <v>91</v>
+      </c>
+      <c r="B10" s="68" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="66" t="s">
         <v>92</v>
       </c>
-      <c r="B10" s="68" t="s">
+      <c r="B11" s="68" t="s">
         <v>86</v>
       </c>
     </row>
@@ -3789,15 +6195,19 @@
   <mergeCells count="1">
     <mergeCell ref="A1:B1"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="F3" r:id="rId1" xr:uid="{81E23815-69B8-4242-AB50-1C2368E4C629}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{5A2D02A3-48EF-4F4D-BEF7-3AFA8E93191C}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{3B1A44A0-3BF5-4702-9671-315837E9B8BF}">
           <x14:formula1>
-            <xm:f>'Participation List'!$H$2:$H$3</xm:f>
+            <xm:f>'Participation List'!$I$2:$I$3</xm:f>
           </x14:formula1>
-          <xm:sqref>B7:B10</xm:sqref>
+          <xm:sqref>B8:B11</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -3805,7 +6215,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FC13C54-3B63-4CB8-9E16-128CB2FA3ED9}">
   <dimension ref="A1:B11"/>
   <sheetViews>
@@ -3820,10 +6230,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="17.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A1" s="83" t="s">
+      <c r="A1" s="84" t="s">
         <v>88</v>
       </c>
-      <c r="B1" s="83"/>
+      <c r="B1" s="84"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="66" t="s">
@@ -3846,8 +6256,8 @@
         <v>93</v>
       </c>
       <c r="B4" s="72">
-        <f>COUNTIF('Participation List'!E3:E32, "Autocar")</f>
-        <v>27</v>
+        <f>COUNTIF('Participation List'!F3:F32, "Autocar")</f>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -3916,7 +6326,7 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{55F9CDC8-C5F3-4569-9985-BB238C0C9739}">
           <x14:formula1>
-            <xm:f>'Participation List'!$H$2:$H$3</xm:f>
+            <xm:f>'Participation List'!$I$2:$I$3</xm:f>
           </x14:formula1>
           <xm:sqref>B8:B11</xm:sqref>
         </x14:dataValidation>
@@ -3926,7 +6336,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C9531C7-AE89-44CA-AB26-4463BF4DA6D3}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -3940,7 +6350,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3A6AECF-CF1B-4DDA-8E76-FA75F3154E8C}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -3952,18 +6362,4 @@
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9F22359-FC7F-4C60-A43A-F5055E3A7BE0}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:C3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Modified: grid layout; Added: database structure for MyCabin App
</commit_message>
<xml_diff>
--- a/Event Organizer App/Algorithms/Budget_Calculator.xlsx
+++ b/Event Organizer App/Algorithms/Budget_Calculator.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CabinApp\Cabana_app\Event Organizer App\Algorithms\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27FFA33C-9B98-4F5A-8A14-5F3F2C1BA9E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86304B84-E23E-4B53-B26E-41DDF89F8A98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8595" yWindow="-15870" windowWidth="25440" windowHeight="15390" firstSheet="1" activeTab="4" xr2:uid="{73935AE9-622C-41E0-9B02-D732681E28C4}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="5" xr2:uid="{73935AE9-622C-41E0-9B02-D732681E28C4}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
@@ -1467,7 +1467,7 @@
     <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="155">
+  <cellXfs count="153">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1792,87 +1792,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="36" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="29" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1883,15 +1802,92 @@
     <xf numFmtId="0" fontId="0" fillId="21" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="22" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -1958,36 +1954,6 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
@@ -2077,6 +2043,25 @@
           <c:val>
             <c:numRef>
               <c:f>'Finance Report'!$B$15:$B$19</c:f>
+              <c:numCache>
+                <c:formatCode>_([$€-2]\ * #,##0.00_);_([$€-2]\ * \(#,##0.00\);_([$€-2]\ * "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>700</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>500</c:v>
+                </c:pt>
+              </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
@@ -2167,6 +2152,25 @@
           <c:val>
             <c:numRef>
               <c:f>'Finance Report'!$C$15:$C$19</c:f>
+              <c:numCache>
+                <c:formatCode>_([$€-2]\ * #,##0.00_);_([$€-2]\ * \(#,##0.00\);_([$€-2]\ * "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>700</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1500</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
@@ -2257,6 +2261,25 @@
           <c:val>
             <c:numRef>
               <c:f>'Finance Report'!$D$15:$D$19</c:f>
+              <c:numCache>
+                <c:formatCode>_([$€-2]\ * #,##0.00_);_([$€-2]\ * \(#,##0.00\);_([$€-2]\ * "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>2250</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>900</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1400</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>50</c:v>
+                </c:pt>
+              </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
@@ -2581,36 +2604,6 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
@@ -2645,6 +2638,13 @@
           <c:val>
             <c:numRef>
               <c:f>'Finance Report'!$B$15</c:f>
+              <c:numCache>
+                <c:formatCode>_([$€-2]\ * #,##0.00_);_([$€-2]\ * \(#,##0.00\);_([$€-2]\ * "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>2000</c:v>
+                </c:pt>
+              </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
@@ -2680,6 +2680,13 @@
           <c:val>
             <c:numRef>
               <c:f>'Finance Report'!$C$15</c:f>
+              <c:numCache>
+                <c:formatCode>_([$€-2]\ * #,##0.00_);_([$€-2]\ * \(#,##0.00\);_([$€-2]\ * "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>2000</c:v>
+                </c:pt>
+              </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
@@ -2715,6 +2722,13 @@
           <c:val>
             <c:numRef>
               <c:f>'Finance Report'!$D$15</c:f>
+              <c:numCache>
+                <c:formatCode>_([$€-2]\ * #,##0.00_);_([$€-2]\ * \(#,##0.00\);_([$€-2]\ * "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>2250</c:v>
+                </c:pt>
+              </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
@@ -5569,20 +5583,20 @@
         <v>10000</v>
       </c>
       <c r="D2" s="45"/>
-      <c r="E2" s="120" t="s">
+      <c r="E2" s="126" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="121"/>
+      <c r="F2" s="127"/>
       <c r="G2" s="45"/>
-      <c r="H2" s="120" t="s">
+      <c r="H2" s="126" t="s">
         <v>9</v>
       </c>
-      <c r="I2" s="121"/>
+      <c r="I2" s="127"/>
       <c r="J2" s="45"/>
-      <c r="K2" s="120" t="s">
+      <c r="K2" s="126" t="s">
         <v>10</v>
       </c>
-      <c r="L2" s="121"/>
+      <c r="L2" s="127"/>
       <c r="P2" s="7" t="s">
         <v>13</v>
       </c>
@@ -6687,7 +6701,7 @@
       <c r="D1" s="86" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="129" t="str" cm="1">
+      <c r="F1" s="144" t="str" cm="1">
         <f t="array" ref="F1">INDEX($S$19:$U$19,0,MATCH(MAX($S16:$U16),$S16:$U16,0))</f>
         <v>15-18 Jun</v>
       </c>
@@ -6715,7 +6729,7 @@
       <c r="P1" s="90" t="s">
         <v>2</v>
       </c>
-      <c r="Q1" s="122" t="s">
+      <c r="Q1" s="140" t="s">
         <v>157</v>
       </c>
     </row>
@@ -6730,7 +6744,7 @@
       <c r="D2" s="66" t="s">
         <v>131</v>
       </c>
-      <c r="F2" s="130"/>
+      <c r="F2" s="145"/>
       <c r="G2">
         <v>1</v>
       </c>
@@ -6754,7 +6768,7 @@
       <c r="P2" s="91" t="s">
         <v>131</v>
       </c>
-      <c r="Q2" s="123"/>
+      <c r="Q2" s="141"/>
     </row>
     <row r="3" spans="1:26" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="66" t="s">
@@ -6767,7 +6781,7 @@
       <c r="D3" s="66" t="s">
         <v>131</v>
       </c>
-      <c r="F3" s="130"/>
+      <c r="F3" s="145"/>
       <c r="G3">
         <v>2</v>
       </c>
@@ -6787,7 +6801,7 @@
       <c r="D4" s="66" t="s">
         <v>131</v>
       </c>
-      <c r="F4" s="130"/>
+      <c r="F4" s="145"/>
       <c r="G4">
         <v>3</v>
       </c>
@@ -6810,7 +6824,7 @@
       <c r="Q4" s="78" t="s">
         <v>145</v>
       </c>
-      <c r="R4" s="122" t="s">
+      <c r="R4" s="140" t="s">
         <v>157</v>
       </c>
     </row>
@@ -6823,7 +6837,7 @@
       <c r="D5" s="66" t="s">
         <v>130</v>
       </c>
-      <c r="F5" s="130"/>
+      <c r="F5" s="145"/>
       <c r="G5">
         <v>4</v>
       </c>
@@ -6847,7 +6861,7 @@
       <c r="Q5" s="94" t="s">
         <v>154</v>
       </c>
-      <c r="R5" s="123"/>
+      <c r="R5" s="141"/>
     </row>
     <row r="6" spans="1:26" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="66" t="s">
@@ -6860,7 +6874,7 @@
       <c r="D6" s="66" t="s">
         <v>131</v>
       </c>
-      <c r="F6" s="130"/>
+      <c r="F6" s="145"/>
       <c r="G6">
         <v>5</v>
       </c>
@@ -6882,7 +6896,7 @@
       <c r="D7" s="66" t="s">
         <v>131</v>
       </c>
-      <c r="F7" s="130"/>
+      <c r="F7" s="145"/>
       <c r="G7">
         <v>6</v>
       </c>
@@ -6902,7 +6916,7 @@
       <c r="D8" s="66" t="s">
         <v>131</v>
       </c>
-      <c r="F8" s="130"/>
+      <c r="F8" s="145"/>
       <c r="G8">
         <v>7</v>
       </c>
@@ -6922,7 +6936,7 @@
       <c r="D9" s="66" t="s">
         <v>130</v>
       </c>
-      <c r="F9" s="130"/>
+      <c r="F9" s="145"/>
       <c r="G9">
         <v>8</v>
       </c>
@@ -6942,7 +6956,7 @@
       <c r="D10" s="66" t="s">
         <v>131</v>
       </c>
-      <c r="F10" s="130"/>
+      <c r="F10" s="145"/>
       <c r="G10">
         <v>9</v>
       </c>
@@ -6953,7 +6967,7 @@
       <c r="M10" s="92" t="s">
         <v>158</v>
       </c>
-      <c r="N10" s="122" t="s">
+      <c r="N10" s="140" t="s">
         <v>161</v>
       </c>
     </row>
@@ -6970,7 +6984,7 @@
       <c r="D11" s="66" t="s">
         <v>131</v>
       </c>
-      <c r="F11" s="130"/>
+      <c r="F11" s="145"/>
       <c r="G11">
         <v>10</v>
       </c>
@@ -6981,7 +6995,7 @@
       <c r="M11" s="87" t="s">
         <v>115</v>
       </c>
-      <c r="N11" s="123"/>
+      <c r="N11" s="141"/>
     </row>
     <row r="12" spans="1:26" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="66" t="s">
@@ -6996,7 +7010,7 @@
       <c r="D12" s="66" t="s">
         <v>131</v>
       </c>
-      <c r="F12" s="130"/>
+      <c r="F12" s="145"/>
       <c r="G12">
         <v>11</v>
       </c>
@@ -7008,7 +7022,7 @@
       <c r="T12" s="113"/>
       <c r="U12" s="113"/>
       <c r="V12" s="61"/>
-      <c r="W12" s="124"/>
+      <c r="W12" s="139"/>
     </row>
     <row r="13" spans="1:26" ht="13.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="66"/>
@@ -7021,7 +7035,7 @@
       <c r="D13" s="66" t="s">
         <v>131</v>
       </c>
-      <c r="F13" s="130"/>
+      <c r="F13" s="145"/>
       <c r="G13">
         <v>12</v>
       </c>
@@ -7032,7 +7046,7 @@
       <c r="S13" s="44"/>
       <c r="T13" s="44"/>
       <c r="U13" s="44"/>
-      <c r="W13" s="124"/>
+      <c r="W13" s="139"/>
     </row>
     <row r="14" spans="1:26" ht="13.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="66" t="s">
@@ -7047,7 +7061,7 @@
       <c r="D14" s="66" t="s">
         <v>131</v>
       </c>
-      <c r="F14" s="130"/>
+      <c r="F14" s="145"/>
       <c r="G14">
         <v>13</v>
       </c>
@@ -7055,21 +7069,21 @@
       <c r="I14" s="66"/>
       <c r="J14" s="66"/>
       <c r="K14" s="66"/>
-      <c r="N14" s="134" t="s">
+      <c r="N14" s="131" t="s">
         <v>175</v>
       </c>
-      <c r="O14" s="135"/>
-      <c r="P14" s="135"/>
-      <c r="Q14" s="135"/>
-      <c r="R14" s="135"/>
-      <c r="S14" s="135"/>
-      <c r="T14" s="135"/>
-      <c r="U14" s="136"/>
-      <c r="X14" s="131" t="s">
+      <c r="O14" s="132"/>
+      <c r="P14" s="132"/>
+      <c r="Q14" s="132"/>
+      <c r="R14" s="132"/>
+      <c r="S14" s="132"/>
+      <c r="T14" s="132"/>
+      <c r="U14" s="133"/>
+      <c r="X14" s="128" t="s">
         <v>174</v>
       </c>
-      <c r="Y14" s="132"/>
-      <c r="Z14" s="133"/>
+      <c r="Y14" s="129"/>
+      <c r="Z14" s="130"/>
     </row>
     <row r="15" spans="1:26" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="66"/>
@@ -7082,7 +7096,7 @@
       <c r="D15" s="66" t="s">
         <v>131</v>
       </c>
-      <c r="F15" s="130"/>
+      <c r="F15" s="145"/>
       <c r="G15">
         <v>14</v>
       </c>
@@ -7109,7 +7123,7 @@
       <c r="D16" s="66" t="s">
         <v>131</v>
       </c>
-      <c r="F16" s="130"/>
+      <c r="F16" s="145"/>
       <c r="G16">
         <v>15</v>
       </c>
@@ -7139,7 +7153,7 @@
       <c r="D17" s="66" t="s">
         <v>131</v>
       </c>
-      <c r="F17" s="130"/>
+      <c r="F17" s="145"/>
       <c r="G17">
         <v>16</v>
       </c>
@@ -7161,7 +7175,7 @@
       <c r="D18" s="66" t="s">
         <v>131</v>
       </c>
-      <c r="F18" s="130"/>
+      <c r="F18" s="145"/>
       <c r="G18">
         <v>17</v>
       </c>
@@ -7169,10 +7183,10 @@
       <c r="I18" s="66"/>
       <c r="J18" s="66"/>
       <c r="K18" s="66"/>
-      <c r="N18" s="127" t="s">
+      <c r="N18" s="136" t="s">
         <v>162</v>
       </c>
-      <c r="O18" s="128"/>
+      <c r="O18" s="137"/>
       <c r="P18" s="103"/>
       <c r="Q18" s="63"/>
       <c r="S18" s="118" t="str">
@@ -7210,7 +7224,7 @@
       <c r="D19" s="66" t="s">
         <v>131</v>
       </c>
-      <c r="F19" s="130"/>
+      <c r="F19" s="145"/>
       <c r="G19">
         <v>18</v>
       </c>
@@ -7255,7 +7269,7 @@
       <c r="D20" s="66" t="s">
         <v>131</v>
       </c>
-      <c r="F20" s="130"/>
+      <c r="F20" s="145"/>
       <c r="G20">
         <v>19</v>
       </c>
@@ -7292,7 +7306,7 @@
       <c r="D21" s="66" t="s">
         <v>131</v>
       </c>
-      <c r="F21" s="130"/>
+      <c r="F21" s="145"/>
       <c r="G21">
         <v>20</v>
       </c>
@@ -7300,10 +7314,10 @@
       <c r="I21" s="66"/>
       <c r="J21" s="80"/>
       <c r="K21" s="66"/>
-      <c r="N21" s="137" t="s">
+      <c r="N21" s="134" t="s">
         <v>156</v>
       </c>
-      <c r="O21" s="138"/>
+      <c r="O21" s="135"/>
       <c r="S21" s="101"/>
       <c r="T21" s="101"/>
       <c r="U21" s="101"/>
@@ -7324,7 +7338,7 @@
       <c r="D22" s="66" t="s">
         <v>131</v>
       </c>
-      <c r="F22" s="130"/>
+      <c r="F22" s="145"/>
       <c r="G22">
         <v>21</v>
       </c>
@@ -7350,7 +7364,7 @@
       <c r="D23" s="66" t="s">
         <v>130</v>
       </c>
-      <c r="F23" s="130"/>
+      <c r="F23" s="145"/>
       <c r="G23">
         <v>22</v>
       </c>
@@ -7374,7 +7388,7 @@
       <c r="D24" s="66" t="s">
         <v>131</v>
       </c>
-      <c r="F24" s="130"/>
+      <c r="F24" s="145"/>
       <c r="G24">
         <v>23</v>
       </c>
@@ -7406,7 +7420,7 @@
       <c r="D25" s="66" t="s">
         <v>131</v>
       </c>
-      <c r="F25" s="130"/>
+      <c r="F25" s="145"/>
       <c r="G25">
         <v>24</v>
       </c>
@@ -7414,10 +7428,10 @@
       <c r="I25" s="66"/>
       <c r="J25" s="66"/>
       <c r="K25" s="66"/>
-      <c r="N25" s="127" t="s">
+      <c r="N25" s="136" t="s">
         <v>162</v>
       </c>
-      <c r="O25" s="128"/>
+      <c r="O25" s="137"/>
       <c r="Q25" s="116"/>
       <c r="S25" s="101"/>
       <c r="T25" s="101"/>
@@ -7439,7 +7453,7 @@
       <c r="D26" s="66" t="s">
         <v>131</v>
       </c>
-      <c r="F26" s="130"/>
+      <c r="F26" s="145"/>
       <c r="G26">
         <v>25</v>
       </c>
@@ -7474,7 +7488,7 @@
       <c r="D27" s="66" t="s">
         <v>131</v>
       </c>
-      <c r="F27" s="130"/>
+      <c r="F27" s="145"/>
       <c r="G27">
         <v>26</v>
       </c>
@@ -7507,7 +7521,7 @@
       <c r="D28" s="66" t="s">
         <v>131</v>
       </c>
-      <c r="F28" s="130"/>
+      <c r="F28" s="145"/>
       <c r="G28">
         <v>27</v>
       </c>
@@ -7542,7 +7556,7 @@
       <c r="D29" s="66" t="s">
         <v>131</v>
       </c>
-      <c r="F29" s="130"/>
+      <c r="F29" s="145"/>
       <c r="G29">
         <v>28</v>
       </c>
@@ -7550,10 +7564,10 @@
       <c r="I29" s="66"/>
       <c r="J29" s="66"/>
       <c r="K29" s="66"/>
-      <c r="N29" s="125" t="s">
+      <c r="N29" s="142" t="s">
         <v>156</v>
       </c>
-      <c r="O29" s="126"/>
+      <c r="O29" s="143"/>
       <c r="S29" s="101"/>
       <c r="T29" s="101"/>
       <c r="U29" s="101"/>
@@ -7572,7 +7586,7 @@
       <c r="D30" s="66" t="s">
         <v>131</v>
       </c>
-      <c r="F30" s="130"/>
+      <c r="F30" s="145"/>
       <c r="G30">
         <v>29</v>
       </c>
@@ -7580,8 +7594,8 @@
       <c r="I30" s="66"/>
       <c r="J30" s="66"/>
       <c r="K30" s="66"/>
-      <c r="N30" s="124"/>
-      <c r="O30" s="124"/>
+      <c r="N30" s="139"/>
+      <c r="O30" s="139"/>
       <c r="P30" s="63"/>
       <c r="Q30" s="63"/>
       <c r="S30" s="101"/>
@@ -7604,7 +7618,7 @@
       <c r="D31" s="66" t="s">
         <v>131</v>
       </c>
-      <c r="F31" s="130"/>
+      <c r="F31" s="145"/>
       <c r="G31">
         <v>30</v>
       </c>
@@ -7635,7 +7649,7 @@
         <f>COUNTA(C2:C31)</f>
         <v>21</v>
       </c>
-      <c r="F32" s="130"/>
+      <c r="F32" s="145"/>
       <c r="H32" s="95">
         <v>14</v>
       </c>
@@ -7690,8 +7704,8 @@
       <c r="B35" s="82"/>
       <c r="C35" s="82"/>
       <c r="F35" s="84"/>
-      <c r="N35" s="139"/>
-      <c r="O35" s="139"/>
+      <c r="N35" s="138"/>
+      <c r="O35" s="138"/>
       <c r="S35" s="101"/>
       <c r="T35" s="101"/>
       <c r="U35" s="101"/>
@@ -7760,12 +7774,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="X14:Z14"/>
-    <mergeCell ref="N14:U14"/>
-    <mergeCell ref="N21:O21"/>
-    <mergeCell ref="N18:O18"/>
-    <mergeCell ref="N35:O35"/>
-    <mergeCell ref="N30:O30"/>
     <mergeCell ref="R4:R5"/>
     <mergeCell ref="W12:W13"/>
     <mergeCell ref="N29:O29"/>
@@ -7773,6 +7781,12 @@
     <mergeCell ref="F1:F32"/>
     <mergeCell ref="Q1:Q2"/>
     <mergeCell ref="N10:N11"/>
+    <mergeCell ref="X14:Z14"/>
+    <mergeCell ref="N14:U14"/>
+    <mergeCell ref="N21:O21"/>
+    <mergeCell ref="N18:O18"/>
+    <mergeCell ref="N35:O35"/>
+    <mergeCell ref="N30:O30"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <dataValidations count="1">
@@ -7816,13 +7830,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B1" s="142" t="s">
+      <c r="B1" s="148" t="s">
         <v>55</v>
       </c>
-      <c r="C1" s="143"/>
-      <c r="D1" s="143"/>
-      <c r="E1" s="143"/>
-      <c r="F1" s="144"/>
+      <c r="C1" s="149"/>
+      <c r="D1" s="149"/>
+      <c r="E1" s="149"/>
+      <c r="F1" s="150"/>
       <c r="H1" s="61" t="s">
         <v>61</v>
       </c>
@@ -7837,10 +7851,10 @@
       <c r="A2" s="68" t="s">
         <v>140</v>
       </c>
-      <c r="B2" s="141" t="s">
+      <c r="B2" s="147" t="s">
         <v>54</v>
       </c>
-      <c r="C2" s="141"/>
+      <c r="C2" s="147"/>
       <c r="D2" s="66" t="s">
         <v>56</v>
       </c>
@@ -7865,10 +7879,10 @@
         <f>DateVoting!$F$1</f>
         <v>15-18 Jun</v>
       </c>
-      <c r="B3" s="140" t="s">
+      <c r="B3" s="146" t="s">
         <v>115</v>
       </c>
-      <c r="C3" s="140"/>
+      <c r="C3" s="146"/>
       <c r="D3" s="66" t="s">
         <v>86</v>
       </c>
@@ -7893,10 +7907,10 @@
         <f>DateVoting!$F$1</f>
         <v>15-18 Jun</v>
       </c>
-      <c r="B4" s="140" t="s">
+      <c r="B4" s="146" t="s">
         <v>116</v>
       </c>
-      <c r="C4" s="140"/>
+      <c r="C4" s="146"/>
       <c r="D4" s="66" t="s">
         <v>86</v>
       </c>
@@ -7924,10 +7938,10 @@
         <f>DateVoting!$F$1</f>
         <v>15-18 Jun</v>
       </c>
-      <c r="B5" s="140" t="s">
+      <c r="B5" s="146" t="s">
         <v>117</v>
       </c>
-      <c r="C5" s="140"/>
+      <c r="C5" s="146"/>
       <c r="D5" s="66" t="s">
         <v>85</v>
       </c>
@@ -7952,10 +7966,10 @@
         <f>DateVoting!$F$1</f>
         <v>15-18 Jun</v>
       </c>
-      <c r="B6" s="140" t="s">
+      <c r="B6" s="146" t="s">
         <v>118</v>
       </c>
-      <c r="C6" s="140"/>
+      <c r="C6" s="146"/>
       <c r="D6" s="66" t="s">
         <v>86</v>
       </c>
@@ -7980,10 +7994,10 @@
         <f>DateVoting!$F$1</f>
         <v>15-18 Jun</v>
       </c>
-      <c r="B7" s="140" t="s">
+      <c r="B7" s="146" t="s">
         <v>119</v>
       </c>
-      <c r="C7" s="140"/>
+      <c r="C7" s="146"/>
       <c r="D7" s="66" t="s">
         <v>85</v>
       </c>
@@ -8002,10 +8016,10 @@
         <f>DateVoting!$F$1</f>
         <v>15-18 Jun</v>
       </c>
-      <c r="B8" s="140" t="s">
+      <c r="B8" s="146" t="s">
         <v>120</v>
       </c>
-      <c r="C8" s="140"/>
+      <c r="C8" s="146"/>
       <c r="D8" s="66" t="s">
         <v>85</v>
       </c>
@@ -8024,10 +8038,10 @@
         <f>DateVoting!$F$1</f>
         <v>15-18 Jun</v>
       </c>
-      <c r="B9" s="140" t="s">
+      <c r="B9" s="146" t="s">
         <v>121</v>
       </c>
-      <c r="C9" s="140"/>
+      <c r="C9" s="146"/>
       <c r="D9" s="66" t="s">
         <v>86</v>
       </c>
@@ -8046,10 +8060,10 @@
         <f>DateVoting!$F$1</f>
         <v>15-18 Jun</v>
       </c>
-      <c r="B10" s="140" t="s">
+      <c r="B10" s="146" t="s">
         <v>122</v>
       </c>
-      <c r="C10" s="140"/>
+      <c r="C10" s="146"/>
       <c r="D10" s="66" t="s">
         <v>86</v>
       </c>
@@ -8068,10 +8082,10 @@
         <f>DateVoting!$F$1</f>
         <v>15-18 Jun</v>
       </c>
-      <c r="B11" s="140" t="s">
+      <c r="B11" s="146" t="s">
         <v>123</v>
       </c>
-      <c r="C11" s="140"/>
+      <c r="C11" s="146"/>
       <c r="D11" s="66" t="s">
         <v>86</v>
       </c>
@@ -8090,10 +8104,10 @@
         <f>DateVoting!$F$1</f>
         <v>15-18 Jun</v>
       </c>
-      <c r="B12" s="140" t="s">
+      <c r="B12" s="146" t="s">
         <v>94</v>
       </c>
-      <c r="C12" s="140"/>
+      <c r="C12" s="146"/>
       <c r="D12" s="66" t="s">
         <v>85</v>
       </c>
@@ -8112,10 +8126,10 @@
         <f>DateVoting!$F$1</f>
         <v>15-18 Jun</v>
       </c>
-      <c r="B13" s="140" t="s">
+      <c r="B13" s="146" t="s">
         <v>95</v>
       </c>
-      <c r="C13" s="140"/>
+      <c r="C13" s="146"/>
       <c r="D13" s="66" t="s">
         <v>86</v>
       </c>
@@ -8134,10 +8148,10 @@
         <f>DateVoting!$F$1</f>
         <v>15-18 Jun</v>
       </c>
-      <c r="B14" s="140" t="s">
+      <c r="B14" s="146" t="s">
         <v>96</v>
       </c>
-      <c r="C14" s="140"/>
+      <c r="C14" s="146"/>
       <c r="D14" s="66" t="s">
         <v>86</v>
       </c>
@@ -8156,10 +8170,10 @@
         <f>DateVoting!$F$1</f>
         <v>15-18 Jun</v>
       </c>
-      <c r="B15" s="140" t="s">
+      <c r="B15" s="146" t="s">
         <v>97</v>
       </c>
-      <c r="C15" s="140"/>
+      <c r="C15" s="146"/>
       <c r="D15" s="66" t="s">
         <v>86</v>
       </c>
@@ -8178,10 +8192,10 @@
         <f>DateVoting!$F$1</f>
         <v>15-18 Jun</v>
       </c>
-      <c r="B16" s="140" t="s">
+      <c r="B16" s="146" t="s">
         <v>98</v>
       </c>
-      <c r="C16" s="140"/>
+      <c r="C16" s="146"/>
       <c r="D16" s="66" t="s">
         <v>85</v>
       </c>
@@ -8200,10 +8214,10 @@
         <f>DateVoting!$F$1</f>
         <v>15-18 Jun</v>
       </c>
-      <c r="B17" s="140" t="s">
+      <c r="B17" s="146" t="s">
         <v>99</v>
       </c>
-      <c r="C17" s="140"/>
+      <c r="C17" s="146"/>
       <c r="D17" s="66" t="s">
         <v>85</v>
       </c>
@@ -8222,10 +8236,10 @@
         <f>DateVoting!$F$1</f>
         <v>15-18 Jun</v>
       </c>
-      <c r="B18" s="140" t="s">
+      <c r="B18" s="146" t="s">
         <v>100</v>
       </c>
-      <c r="C18" s="140"/>
+      <c r="C18" s="146"/>
       <c r="D18" s="66" t="s">
         <v>85</v>
       </c>
@@ -8244,10 +8258,10 @@
         <f>DateVoting!$F$1</f>
         <v>15-18 Jun</v>
       </c>
-      <c r="B19" s="140" t="s">
+      <c r="B19" s="146" t="s">
         <v>101</v>
       </c>
-      <c r="C19" s="140"/>
+      <c r="C19" s="146"/>
       <c r="D19" s="66" t="s">
         <v>86</v>
       </c>
@@ -8266,10 +8280,10 @@
         <f>DateVoting!$F$1</f>
         <v>15-18 Jun</v>
       </c>
-      <c r="B20" s="140" t="s">
+      <c r="B20" s="146" t="s">
         <v>102</v>
       </c>
-      <c r="C20" s="140"/>
+      <c r="C20" s="146"/>
       <c r="D20" s="66" t="s">
         <v>86</v>
       </c>
@@ -8288,10 +8302,10 @@
         <f>DateVoting!$F$1</f>
         <v>15-18 Jun</v>
       </c>
-      <c r="B21" s="140" t="s">
+      <c r="B21" s="146" t="s">
         <v>103</v>
       </c>
-      <c r="C21" s="140"/>
+      <c r="C21" s="146"/>
       <c r="D21" s="66" t="s">
         <v>86</v>
       </c>
@@ -8310,10 +8324,10 @@
         <f>DateVoting!$F$1</f>
         <v>15-18 Jun</v>
       </c>
-      <c r="B22" s="140" t="s">
+      <c r="B22" s="146" t="s">
         <v>104</v>
       </c>
-      <c r="C22" s="140"/>
+      <c r="C22" s="146"/>
       <c r="D22" s="66" t="s">
         <v>86</v>
       </c>
@@ -8332,10 +8346,10 @@
         <f>DateVoting!$F$1</f>
         <v>15-18 Jun</v>
       </c>
-      <c r="B23" s="140" t="s">
+      <c r="B23" s="146" t="s">
         <v>105</v>
       </c>
-      <c r="C23" s="140"/>
+      <c r="C23" s="146"/>
       <c r="D23" s="66" t="s">
         <v>85</v>
       </c>
@@ -8354,10 +8368,10 @@
         <f>DateVoting!$F$1</f>
         <v>15-18 Jun</v>
       </c>
-      <c r="B24" s="140" t="s">
+      <c r="B24" s="146" t="s">
         <v>106</v>
       </c>
-      <c r="C24" s="140"/>
+      <c r="C24" s="146"/>
       <c r="D24" s="66" t="s">
         <v>86</v>
       </c>
@@ -8376,10 +8390,10 @@
         <f>DateVoting!$F$1</f>
         <v>15-18 Jun</v>
       </c>
-      <c r="B25" s="140" t="s">
+      <c r="B25" s="146" t="s">
         <v>107</v>
       </c>
-      <c r="C25" s="140"/>
+      <c r="C25" s="146"/>
       <c r="D25" s="66" t="s">
         <v>86</v>
       </c>
@@ -8398,10 +8412,10 @@
         <f>DateVoting!$F$1</f>
         <v>15-18 Jun</v>
       </c>
-      <c r="B26" s="140" t="s">
+      <c r="B26" s="146" t="s">
         <v>108</v>
       </c>
-      <c r="C26" s="140"/>
+      <c r="C26" s="146"/>
       <c r="D26" s="66" t="s">
         <v>86</v>
       </c>
@@ -8420,10 +8434,10 @@
         <f>DateVoting!$F$1</f>
         <v>15-18 Jun</v>
       </c>
-      <c r="B27" s="140" t="s">
+      <c r="B27" s="146" t="s">
         <v>109</v>
       </c>
-      <c r="C27" s="140"/>
+      <c r="C27" s="146"/>
       <c r="D27" s="66" t="s">
         <v>85</v>
       </c>
@@ -8442,10 +8456,10 @@
         <f>DateVoting!$F$1</f>
         <v>15-18 Jun</v>
       </c>
-      <c r="B28" s="140" t="s">
+      <c r="B28" s="146" t="s">
         <v>110</v>
       </c>
-      <c r="C28" s="140"/>
+      <c r="C28" s="146"/>
       <c r="D28" s="66" t="s">
         <v>86</v>
       </c>
@@ -8461,10 +8475,10 @@
         <f>DateVoting!$F$1</f>
         <v>15-18 Jun</v>
       </c>
-      <c r="B29" s="140" t="s">
+      <c r="B29" s="146" t="s">
         <v>111</v>
       </c>
-      <c r="C29" s="140"/>
+      <c r="C29" s="146"/>
       <c r="D29" s="66" t="s">
         <v>86</v>
       </c>
@@ -8480,10 +8494,10 @@
         <f>DateVoting!$F$1</f>
         <v>15-18 Jun</v>
       </c>
-      <c r="B30" s="140" t="s">
+      <c r="B30" s="146" t="s">
         <v>112</v>
       </c>
-      <c r="C30" s="140"/>
+      <c r="C30" s="146"/>
       <c r="D30" s="66" t="s">
         <v>85</v>
       </c>
@@ -8499,10 +8513,10 @@
         <f>DateVoting!$F$1</f>
         <v>15-18 Jun</v>
       </c>
-      <c r="B31" s="140" t="s">
+      <c r="B31" s="146" t="s">
         <v>113</v>
       </c>
-      <c r="C31" s="140"/>
+      <c r="C31" s="146"/>
       <c r="D31" s="66" t="s">
         <v>86</v>
       </c>
@@ -8518,10 +8532,10 @@
         <f>DateVoting!$F$1</f>
         <v>15-18 Jun</v>
       </c>
-      <c r="B32" s="140" t="s">
+      <c r="B32" s="146" t="s">
         <v>114</v>
       </c>
-      <c r="C32" s="140"/>
+      <c r="C32" s="146"/>
       <c r="D32" s="66" t="s">
         <v>86</v>
       </c>
@@ -8534,15 +8548,17 @@
     </row>
   </sheetData>
   <mergeCells count="32">
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B10:C10"/>
     <mergeCell ref="B23:C23"/>
     <mergeCell ref="B12:C12"/>
     <mergeCell ref="B13:C13"/>
@@ -8555,17 +8571,15 @@
     <mergeCell ref="B20:C20"/>
     <mergeCell ref="B21:C21"/>
     <mergeCell ref="B22:C22"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B1:F1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="B28:C28"/>
   </mergeCells>
   <dataValidations count="3">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3:F32" xr:uid="{AD533C06-5237-486A-8404-42C5B3D58852}">
@@ -8603,15 +8617,15 @@
       <c r="A3" s="76" t="s">
         <v>142</v>
       </c>
-      <c r="C3" s="140" t="s">
+      <c r="C3" s="146" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="140"/>
+      <c r="D3" s="146"/>
       <c r="E3" s="77"/>
-      <c r="F3" s="140" t="s">
+      <c r="F3" s="146" t="s">
         <v>141</v>
       </c>
-      <c r="G3" s="140"/>
+      <c r="G3" s="146"/>
       <c r="I3" t="s">
         <v>146</v>
       </c>
@@ -9011,18 +9025,18 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A94A1BE0-93F2-4C18-9D5C-FE2D9F3472AE}">
-  <dimension ref="A1:K36"/>
+  <dimension ref="A1:K35"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.6640625" style="63" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.5546875" style="63" hidden="1" customWidth="1"/>
-    <col min="3" max="3" width="22.88671875" style="63" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="29" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="23.5546875" style="63" customWidth="1"/>
+    <col min="3" max="3" width="22.88671875" style="63" customWidth="1"/>
+    <col min="4" max="4" width="29" customWidth="1"/>
     <col min="5" max="5" width="16.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.88671875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
@@ -9032,40 +9046,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A1" s="145" t="s">
+      <c r="A1" s="151" t="s">
         <v>88</v>
       </c>
-      <c r="B1" s="145"/>
-      <c r="C1" s="145"/>
+      <c r="B1" s="151"/>
+      <c r="C1" s="151"/>
       <c r="D1" s="62"/>
-      <c r="E1" s="145" t="s">
+      <c r="E1" s="151" t="s">
         <v>46</v>
       </c>
-      <c r="F1" s="145"/>
-      <c r="G1" s="145"/>
-      <c r="I1" s="145" t="s">
+      <c r="F1" s="151"/>
+      <c r="G1" s="151"/>
+      <c r="I1" s="151" t="s">
         <v>47</v>
       </c>
-      <c r="J1" s="145"/>
-      <c r="K1" s="145"/>
+      <c r="J1" s="151"/>
+      <c r="K1" s="151"/>
     </row>
     <row r="2" spans="1:11" ht="22.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="146" t="str">
+      <c r="A2" s="152" t="str">
         <f>Location!B2</f>
         <v>Pensiunea Valea Zanelor</v>
       </c>
-      <c r="B2" s="146"/>
-      <c r="C2" s="146"/>
-      <c r="E2" s="146" t="s">
+      <c r="B2" s="152"/>
+      <c r="C2" s="152"/>
+      <c r="E2" s="152" t="s">
         <v>51</v>
       </c>
-      <c r="F2" s="146"/>
-      <c r="G2" s="146"/>
-      <c r="I2" s="146" t="s">
+      <c r="F2" s="152"/>
+      <c r="G2" s="152"/>
+      <c r="I2" s="152" t="s">
         <v>52</v>
       </c>
-      <c r="J2" s="146"/>
-      <c r="K2" s="146"/>
+      <c r="J2" s="152"/>
+      <c r="K2" s="152"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="64" t="s">
@@ -9251,11 +9265,11 @@
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B12" s="154" t="str">
+      <c r="B12" s="125" t="str">
         <f>A2</f>
         <v>Pensiunea Valea Zanelor</v>
       </c>
-      <c r="C12" s="154" t="str">
+      <c r="C12" s="125" t="str">
         <f>E2</f>
         <v>Pensiunea Vila Boierilor</v>
       </c>
@@ -9394,34 +9408,29 @@
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B32" s="153" t="s">
+      <c r="B32" s="124" t="s">
         <v>178</v>
       </c>
-      <c r="C32" s="153"/>
+      <c r="C32" s="124"/>
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B33" s="147" t="s">
+      <c r="B33" s="120" t="s">
         <v>182</v>
       </c>
-      <c r="C33" s="147"/>
-      <c r="D33" s="148"/>
+      <c r="C33" s="120"/>
+      <c r="D33" s="121"/>
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B34" s="149" t="s">
+      <c r="B34" s="122" t="s">
         <v>183</v>
       </c>
-      <c r="C34" s="149"/>
+      <c r="C34" s="122"/>
     </row>
     <row r="35" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B35" s="150" t="s">
+      <c r="B35" s="123" t="s">
         <v>184</v>
       </c>
-      <c r="C35" s="150"/>
-    </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B36" s="151"/>
-      <c r="C36" s="151"/>
-      <c r="D36" s="152"/>
+      <c r="C35" s="123"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -9452,8 +9461,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACE780CE-1C58-49A2-9B78-7393F891FAAC}">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -9465,10 +9474,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A1" s="145" t="s">
+      <c r="A1" s="151" t="s">
         <v>88</v>
       </c>
-      <c r="B1" s="145"/>
+      <c r="B1" s="151"/>
       <c r="C1" s="70"/>
     </row>
     <row r="2" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.25">
@@ -9611,10 +9620,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="17.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A1" s="145" t="s">
+      <c r="A1" s="151" t="s">
         <v>88</v>
       </c>
-      <c r="B1" s="145"/>
+      <c r="B1" s="151"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="66" t="s">

</xml_diff>